<commit_message>
Code changes for Archived Results and append to day result file and more regression cases
</commit_message>
<xml_diff>
--- a/LYNX_Automation/src/test/resources/TestData/Test_Data.xlsx
+++ b/LYNX_Automation/src/test/resources/TestData/Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X023840\git\Fastwire\LYNX_Automation\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C512407A-B04E-4362-9476-3459F96D4DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34A9C05-8ABE-4BDD-899F-8FCC4C64F8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="179">
   <si>
     <t>RunTest</t>
   </si>
@@ -471,9 +471,6 @@
     <t>Aim of the script is to verify whether company and RIC are displayed in Story body</t>
   </si>
   <si>
-    <t>Aim of the Scirpt  is to verify the associated Product and topic codes are displayed when select multiple RIC's in Alert Editor</t>
-  </si>
-  <si>
     <t>FW_UI_0035</t>
   </si>
   <si>
@@ -487,13 +484,100 @@
   </si>
   <si>
     <t>Verify_Display_Metadata_RIC</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>FW_UI_0037</t>
+  </si>
+  <si>
+    <t>Aim of the script is to verify whether story ID column is present or not in Story list.</t>
+  </si>
+  <si>
+    <t>Verify_Alert_Publish</t>
+  </si>
+  <si>
+    <t>FW_UI_0038</t>
+  </si>
+  <si>
+    <t>Verify_StoryID_Format</t>
+  </si>
+  <si>
+    <t>FW_UI_0039</t>
+  </si>
+  <si>
+    <t>Aim of the script is to verify whether story ID format in 1 to 999 range.</t>
+  </si>
+  <si>
+    <t>Verify_Multiplecodes</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>Topics</t>
+  </si>
+  <si>
+    <t>Aim of the Script  is to verify the associated Product and topic codes are displayed when select multiple RIC's in Alert Editor</t>
+  </si>
+  <si>
+    <t>Aim of the Script  is to verify whether the alert is published  or not using alert editor.</t>
+  </si>
+  <si>
+    <t>Aim of the Script  is to verify whether user is able to add multiple product codes in alert editor.</t>
+  </si>
+  <si>
+    <t>Aim of the Script  is to verify whether user is able to add multiple topic codes in alert editor.</t>
+  </si>
+  <si>
+    <t>FW_UI_0040</t>
+  </si>
+  <si>
+    <t>FW_UI_0041</t>
+  </si>
+  <si>
+    <t>Verify_USN</t>
+  </si>
+  <si>
+    <t>Aim of the Script  is to verify whether publish is enabled or not when alert text is not entered in alert editor.</t>
+  </si>
+  <si>
+    <t>Aim of the Script  is to verify whether user is able get the USN when click on the 'Get' button in alert editor.</t>
+  </si>
+  <si>
+    <t>FW_UI_0042</t>
+  </si>
+  <si>
+    <t>Aim of the Scirpt  is to verify that Publish button should be enabled when alert text is more than 150 characters in alert editor.</t>
+  </si>
+  <si>
+    <t>FW_UI_0043</t>
+  </si>
+  <si>
+    <t>Publish,Test Publish</t>
+  </si>
+  <si>
+    <t>BlankAlerttext,Test Publish</t>
+  </si>
+  <si>
+    <t>Publish,Test Publish This text is to confirm whether headline publish happens successfully or not for more than one hunderd and fifty characters alert text entered by user</t>
+  </si>
+  <si>
+    <t>Aim of the Scirpt  is to verify whether Publish button is enabled or not when alert text is 50 characters in alert editor.</t>
+  </si>
+  <si>
+    <t>FW_UI_0044</t>
+  </si>
+  <si>
+    <t>Publish,Test Publish FiftyCharacters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -507,6 +591,11 @@
       <b/>
       <sz val="10"/>
       <color indexed="17"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -613,7 +702,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -651,6 +740,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -948,7 +1040,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CBB49106-BC95-4A00-9B23-0E30E5D20288}" name="Table2" displayName="Table2" ref="A2:F43" headerRowCount="0" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CBB49106-BC95-4A00-9B23-0E30E5D20288}" name="Table2" displayName="Table2" ref="A2:F51" headerRowCount="0" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E8C12C75-5AB5-4A43-A3C6-442932DE8960}" name="Column1" headerRowDxfId="11" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{2D0C15F7-7463-4837-A664-2CE60CA101D5}" name="Column2" headerRowDxfId="9" dataDxfId="8"/>
@@ -1283,10 +1375,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2094,36 +2186,34 @@
         <v>143</v>
       </c>
       <c r="C41" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>148</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="F41" s="9" t="s">
-        <v>144</v>
+      <c r="F41" s="11" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="s">
-        <v>10</v>
+      <c r="A42" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>149</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D42" s="5"/>
       <c r="E42" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="F42" s="9" t="s">
-        <v>145</v>
+      <c r="F42" s="6" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2131,12 +2221,178 @@
         <v>31</v>
       </c>
       <c r="B43" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D43" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="9"/>
+      <c r="E43" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>176</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
New cases 25 Nov
</commit_message>
<xml_diff>
--- a/LYNX_Automation/src/test/resources/TestData/Test_Data.xlsx
+++ b/LYNX_Automation/src/test/resources/TestData/Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X023840\git\Fastwire_Sikuli\LYNX_Automation\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93CC39C-D8C9-4AF9-9A40-21484C4CDA03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70184792-9A75-48FB-B1BA-0EC91AF1EA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="360">
   <si>
     <t>RunTest</t>
   </si>
@@ -867,9 +867,6 @@
     <t>YES,Publish,TEST PUBLISH THIS TEST CASE IS TO TEST WHETHER TWO HUNDRED CHARACTERS ARE ALLOWED OR NOT FOR PUBLISHING THE ALERTS SUCCESSFULLY NOT THIS TEST CASE IS TO TEST WHETHER TWO HUNDRED,TESTUSN</t>
   </si>
   <si>
-    <t>YES,PlaceHolder,Test Publish,TESTUSN</t>
-  </si>
-  <si>
     <t>YES,Publish,Test Publish,123456789</t>
   </si>
   <si>
@@ -1048,6 +1045,75 @@
   </si>
   <si>
     <t>Publish,Test Publish,TESTUSN,Turkish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aim of the Script is to verify that user should not be able to publish an alert with incomplete placeholders (with incomplete company and RIC), so that I do not publish out an incomplete alert </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aim of the Script is to verify that user should not be able to publish an alert with incomplete placeholders (with an incomplete RIC), so that I do not publish out an incomplete alert </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aim of the Script is to verify that user should not be able to publish an alert with incomplete placeholders (with an incomplete Company), so that I do not publish out an incomplete alert </t>
+  </si>
+  <si>
+    <t>FW_UI_0098</t>
+  </si>
+  <si>
+    <t>FW_UI_0099</t>
+  </si>
+  <si>
+    <t>FW_UI_0100</t>
+  </si>
+  <si>
+    <t>FW_UI_0101</t>
+  </si>
+  <si>
+    <t>FW_UI_0102</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>YES,PlaceHolder,Test Publish~,TESTUSN</t>
+  </si>
+  <si>
+    <t>YES,PlaceHolder,~company~ ~ric~ - SALES AND REVENUES WERE UP $1.780 BLN FROM Q1 OF 2007. SALES VOLUME IMPROVED $1.087,TESTUSN</t>
+  </si>
+  <si>
+    <t>YES,PlaceHolder,~company~ ric - SALES AND REVENUES WERE UP $1.780 BLN FROM Q1 OF 2018. SALES VOLUME IMPROVED,TESTUSN</t>
+  </si>
+  <si>
+    <t>YES,PlaceHolder,Company ~ric~ - SALES AND REVENUES WERE UP $1.780 BLN FROM Q1 OF 2007. SALES VOLUME IMPROVED,TESTUSN</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to verify whether user is able to add multiple product codes in alert editor and publish</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to verify whether user is able to add multiple topic codes in alert editor and publish</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to verify whether user is able to add multiple RICs in alert editor and publish</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to verify whether user is able to add multiple named items in alert editor and publish</t>
+  </si>
+  <si>
+    <t>FW_UI_0103</t>
+  </si>
+  <si>
+    <t>FW_UI_0104</t>
+  </si>
+  <si>
+    <t>Products,SCAN;UKP;SUDB;HX;SUKP,Publish</t>
+  </si>
+  <si>
+    <t>Topics,SASIAE;SANPRO;HAND;HARW;HACK,Publish</t>
+  </si>
+  <si>
+    <t>NamedItems,ABS/;AB/CN,Publish</t>
+  </si>
+  <si>
+    <t>RICS,H.N;D11.HN,Publish</t>
   </si>
 </sst>
 </file>
@@ -1211,48 +1277,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="17"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1419,6 +1443,48 @@
       </fill>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="17"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1433,14 +1499,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CBB49106-BC95-4A00-9B23-0E30E5D20288}" name="Table2" displayName="Table2" ref="A1:F104" totalsRowShown="0" headerRowDxfId="0" dataDxfId="10" headerRowBorderDxfId="1" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CBB49106-BC95-4A00-9B23-0E30E5D20288}" name="Table2" displayName="Table2" ref="A1:F111" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E8C12C75-5AB5-4A43-A3C6-442932DE8960}" name="RunTest" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{2D0C15F7-7463-4837-A664-2CE60CA101D5}" name="TC_ID" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{7C8347B6-FF57-42E1-A6C2-EC27070A40D0}" name="ScriptName" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{EE0534CE-1AD7-4FF9-85D0-3AE501688863}" name="Parameters" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{D9E527CD-0865-44E9-A462-CB70BB730775}" name="Class Name" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{8264D975-498F-4ED6-8B84-152D38F182B3}" name="Description" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{E8C12C75-5AB5-4A43-A3C6-442932DE8960}" name="RunTest" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{2D0C15F7-7463-4837-A664-2CE60CA101D5}" name="TC_ID" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{7C8347B6-FF57-42E1-A6C2-EC27070A40D0}" name="ScriptName" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{EE0534CE-1AD7-4FF9-85D0-3AE501688863}" name="Parameters" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{D9E527CD-0865-44E9-A462-CB70BB730775}" name="Class Name" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{8264D975-498F-4ED6-8B84-152D38F182B3}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1768,10 +1834,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F104"/>
+  <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D110" sqref="D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2858,7 +2924,7 @@
         <v>152</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>277</v>
+        <v>346</v>
       </c>
       <c r="E55" s="7" t="s">
         <v>107</v>
@@ -2878,7 +2944,7 @@
         <v>152</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E56" s="7" t="s">
         <v>107</v>
@@ -2898,7 +2964,7 @@
         <v>152</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E57" s="7" t="s">
         <v>107</v>
@@ -2918,7 +2984,7 @@
         <v>152</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E58" s="7" t="s">
         <v>107</v>
@@ -2938,7 +3004,7 @@
         <v>152</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E59" s="7" t="s">
         <v>107</v>
@@ -2958,7 +3024,7 @@
         <v>152</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E60" s="7" t="s">
         <v>107</v>
@@ -2998,7 +3064,7 @@
         <v>152</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E62" s="7" t="s">
         <v>107</v>
@@ -3492,19 +3558,19 @@
         <v>30</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C87" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F87" s="10" t="s">
         <v>283</v>
-      </c>
-      <c r="D87" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="E87" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="F87" s="10" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3512,19 +3578,19 @@
         <v>30</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E88" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F88" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3532,19 +3598,19 @@
         <v>30</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E89" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F89" s="10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3552,19 +3618,19 @@
         <v>30</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E90" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F90" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3572,19 +3638,19 @@
         <v>30</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E91" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F91" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3592,19 +3658,19 @@
         <v>30</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E92" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F92" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3612,19 +3678,19 @@
         <v>30</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E93" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F93" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3632,19 +3698,19 @@
         <v>30</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E94" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F94" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3652,19 +3718,19 @@
         <v>30</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E95" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F95" s="10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3672,19 +3738,19 @@
         <v>30</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E96" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F96" s="10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3692,19 +3758,19 @@
         <v>30</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E97" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F97" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3712,19 +3778,19 @@
         <v>30</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D98" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E98" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F98" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3732,19 +3798,19 @@
         <v>30</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D99" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E99" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F99" s="10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3752,19 +3818,19 @@
         <v>30</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D100" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E100" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F100" s="10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3772,19 +3838,19 @@
         <v>30</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E101" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F101" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3792,19 +3858,19 @@
         <v>30</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D102" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E102" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F102" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3812,19 +3878,19 @@
         <v>30</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D103" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E103" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F103" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3832,19 +3898,159 @@
         <v>30</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D104" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="E104" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F104" s="10" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="E105" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F105" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="E104" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="F104" s="10" t="s">
-        <v>303</v>
+    </row>
+    <row r="106" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D106" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="E106" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F106" s="6" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D107" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="E107" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D108" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F108" s="10" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F109" s="10" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="E110" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F110" s="10" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="E111" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F111" s="10" t="s">
+        <v>353</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Regression Cases 28th Nov
</commit_message>
<xml_diff>
--- a/LYNX_Automation/src/test/resources/TestData/Test_Data.xlsx
+++ b/LYNX_Automation/src/test/resources/TestData/Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X023840\git\Fastwire_Sikuli\LYNX_Automation\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70184792-9A75-48FB-B1BA-0EC91AF1EA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25C1E2C-5EF1-411C-922C-B8655E51D193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="400">
   <si>
     <t>RunTest</t>
   </si>
@@ -846,9 +846,6 @@
     <t>Aim of the Script  is to verify whether USN filed is taking alpha numerics or not in alert editor.</t>
   </si>
   <si>
-    <t>YES,Publish,Test Publish</t>
-  </si>
-  <si>
     <t>YES,BlankAlerttext,Test Publish,TESTUSN</t>
   </si>
   <si>
@@ -1071,9 +1068,6 @@
     <t>FW_UI_0102</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>YES,PlaceHolder,Test Publish~,TESTUSN</t>
   </si>
   <si>
@@ -1114,6 +1108,132 @@
   </si>
   <si>
     <t>RICS,H.N;D11.HN,Publish</t>
+  </si>
+  <si>
+    <t>Verify_Headline_Search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aim of the Script is to verify that user should be able to search the story with full headline text </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aim of the Script is to verify that user should be able to search the story with part of the headline text </t>
+  </si>
+  <si>
+    <t>Aim of the Script is to verify that user should be able to search the story with single character</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to verify that user should be able to search the story with Story ID</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to verify that user should be able to search the story with number when it is part of headline text.</t>
+  </si>
+  <si>
+    <t>FW_UI_0105</t>
+  </si>
+  <si>
+    <t>FW_UI_0106</t>
+  </si>
+  <si>
+    <t>FW_UI_0107</t>
+  </si>
+  <si>
+    <t>FW_UI_0108</t>
+  </si>
+  <si>
+    <t>FW_UI_0109</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>"438"</t>
+  </si>
+  <si>
+    <t>"4"</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>ny 6</t>
+  </si>
+  <si>
+    <t>FW_UI_0110</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to verify that user should be able to search the story with alphanumeric word (part of the headline text).</t>
+  </si>
+  <si>
+    <t>FW_UI_0111</t>
+  </si>
+  <si>
+    <t>Aim of the Script  is to verify that user should be able to quick publish the story using shortcut key (F12)</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to verify whether the alert is published or not using Shift+F12 shortcut key</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to verify whether able to publish an alert that is being edited or not using (Shift+F12) shortcut key</t>
+  </si>
+  <si>
+    <t>FW_UI_0112</t>
+  </si>
+  <si>
+    <t>FW_UI_0113</t>
+  </si>
+  <si>
+    <t>RICS,H.N,ShortcutPublishF12</t>
+  </si>
+  <si>
+    <t>RICS,H.N,ShortcutPublishSF12</t>
+  </si>
+  <si>
+    <t>FW_UI_0114</t>
+  </si>
+  <si>
+    <t>Verify_RIC_Correction</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to verify RIC correction and Headline publish.</t>
+  </si>
+  <si>
+    <t>H.N,NewTest,Publish</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to verify RIC correction in story header for non english stories with Non-Eng default Product Codes.</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to verify RIC correction in alert editor for non english stories with Non-Eng default codes.</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to verify RIC correction in story header and publish the headline with same RIC for non english stories with Non-Eng default Products.</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to verify RIC correction in alert editor and publish the alert with the same RIC for non english stories with Non-Eng default Products.</t>
+  </si>
+  <si>
+    <t>FW_UI_0115</t>
+  </si>
+  <si>
+    <t>FW_UI_0116</t>
+  </si>
+  <si>
+    <t>FW_UI_0117</t>
+  </si>
+  <si>
+    <t>FW_UI_0118</t>
+  </si>
+  <si>
+    <t>Verify_NonEnglish_Publish_BSKT</t>
+  </si>
+  <si>
+    <t>H.N,Spanish,NoPublish</t>
+  </si>
+  <si>
+    <t>H.N,Spanish,Publish</t>
   </si>
 </sst>
 </file>
@@ -1234,7 +1354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1271,6 +1391,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1499,7 +1622,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CBB49106-BC95-4A00-9B23-0E30E5D20288}" name="Table2" displayName="Table2" ref="A1:F111" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CBB49106-BC95-4A00-9B23-0E30E5D20288}" name="Table2" displayName="Table2" ref="A1:F125" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:F125" xr:uid="{CBB49106-BC95-4A00-9B23-0E30E5D20288}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E8C12C75-5AB5-4A43-A3C6-442932DE8960}" name="RunTest" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{2D0C15F7-7463-4837-A664-2CE60CA101D5}" name="TC_ID" dataDxfId="4"/>
@@ -1834,10 +1958,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F111"/>
+  <dimension ref="A1:F125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2726,7 +2850,7 @@
         <v>152</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>107</v>
@@ -2804,7 +2928,7 @@
         <v>152</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E49" s="7" t="s">
         <v>107</v>
@@ -2824,7 +2948,7 @@
         <v>152</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E50" s="7" t="s">
         <v>107</v>
@@ -2844,7 +2968,7 @@
         <v>152</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E51" s="7" t="s">
         <v>107</v>
@@ -2864,7 +2988,7 @@
         <v>152</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E52" s="7" t="s">
         <v>107</v>
@@ -2884,7 +3008,7 @@
         <v>152</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E53" s="7" t="s">
         <v>107</v>
@@ -2904,7 +3028,7 @@
         <v>152</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E54" s="7" t="s">
         <v>107</v>
@@ -2924,7 +3048,7 @@
         <v>152</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E55" s="7" t="s">
         <v>107</v>
@@ -2944,7 +3068,7 @@
         <v>152</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E56" s="7" t="s">
         <v>107</v>
@@ -2964,7 +3088,7 @@
         <v>152</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E57" s="7" t="s">
         <v>107</v>
@@ -2984,7 +3108,7 @@
         <v>152</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E58" s="7" t="s">
         <v>107</v>
@@ -3004,7 +3128,7 @@
         <v>152</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E59" s="7" t="s">
         <v>107</v>
@@ -3024,7 +3148,7 @@
         <v>152</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E60" s="7" t="s">
         <v>107</v>
@@ -3064,7 +3188,7 @@
         <v>152</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E62" s="7" t="s">
         <v>107</v>
@@ -3558,19 +3682,19 @@
         <v>30</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C87" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F87" s="10" t="s">
         <v>282</v>
-      </c>
-      <c r="D87" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="E87" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="F87" s="10" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3578,19 +3702,19 @@
         <v>30</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E88" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F88" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3598,19 +3722,19 @@
         <v>30</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E89" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F89" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3618,19 +3742,19 @@
         <v>30</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E90" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F90" s="10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3638,19 +3762,19 @@
         <v>30</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E91" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F91" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3658,19 +3782,19 @@
         <v>30</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E92" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F92" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3678,19 +3802,19 @@
         <v>30</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E93" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F93" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3698,19 +3822,19 @@
         <v>30</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E94" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F94" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3718,19 +3842,19 @@
         <v>30</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E95" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F95" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3738,19 +3862,19 @@
         <v>30</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E96" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F96" s="10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3758,19 +3882,19 @@
         <v>30</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E97" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F97" s="10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3778,19 +3902,19 @@
         <v>30</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D98" s="7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E98" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F98" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3798,19 +3922,19 @@
         <v>30</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D99" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E99" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F99" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3818,19 +3942,19 @@
         <v>30</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D100" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E100" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F100" s="10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3838,19 +3962,19 @@
         <v>30</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E101" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F101" s="10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3858,19 +3982,19 @@
         <v>30</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D102" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E102" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F102" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3878,19 +4002,19 @@
         <v>30</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D103" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E103" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F103" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3898,19 +4022,19 @@
         <v>30</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D104" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E104" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F104" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3918,19 +4042,19 @@
         <v>30</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C105" s="7" t="s">
         <v>152</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E105" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F105" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3938,19 +4062,19 @@
         <v>30</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C106" s="7" t="s">
         <v>152</v>
       </c>
       <c r="D106" s="7" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E106" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F106" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3958,19 +4082,19 @@
         <v>30</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C107" s="7" t="s">
         <v>152</v>
       </c>
       <c r="D107" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E107" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F107" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3978,19 +4102,19 @@
         <v>30</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C108" s="7" t="s">
         <v>194</v>
       </c>
       <c r="D108" s="7" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E108" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F108" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3998,39 +4122,39 @@
         <v>30</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C109" s="7" t="s">
         <v>194</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E109" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F109" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
-        <v>345</v>
+        <v>30</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C110" s="7" t="s">
         <v>194</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E110" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F110" s="10" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4038,19 +4162,299 @@
         <v>30</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>194</v>
       </c>
       <c r="D111" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="E111" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F111" s="10" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="C112" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="E111" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="F111" s="10" t="s">
-        <v>353</v>
+      <c r="D112" s="13" t="s">
+        <v>373</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F112" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F113" s="5" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F114" s="5" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="D115" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="E115" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F115" s="5" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="D116" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F116" s="7" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="C117" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="D117" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F117" s="8" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D118" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="E118" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F118" s="8" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="E119" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F119" s="6" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="C120" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D120" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="E120" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F120" s="8" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="C121" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="D121" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="E121" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F121" s="6" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="D122" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="E122" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F122" s="8" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="D123" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="E123" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F123" s="8" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="D124" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="E124" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F124" s="8" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="D125" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="E125" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F125" s="8" t="s">
+        <v>392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Live Feeds and full Search Screen test cases
</commit_message>
<xml_diff>
--- a/LYNX_Automation/src/test/resources/TestData/Test_Data.xlsx
+++ b/LYNX_Automation/src/test/resources/TestData/Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X023840\git\Fastwire_Sikuli\LYNX_Automation\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BF891B-BB5D-43AB-B0B2-8C9E7C8F8294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE8D4F1-658F-4630-84D3-AB4B51FB90E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="497">
   <si>
     <t>RunTest</t>
   </si>
@@ -1327,6 +1327,204 @@
   </si>
   <si>
     <t>YES,HIGHCONTRASTQUICKPUBLISH,TEST PUBLISH HIGHCONTRASTQUICKPUBLISH,TESTUSN</t>
+  </si>
+  <si>
+    <t>HIGHCONTRAST</t>
+  </si>
+  <si>
+    <t>NORMAL</t>
+  </si>
+  <si>
+    <t>H.N,NewTest,HCPublish</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to verify RIC correction and publish alert with same RIC in Alert Editor for high contrast mode.</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to verify RIC correction and Headline publish for high contrast mode.</t>
+  </si>
+  <si>
+    <t>FW_UI_0130</t>
+  </si>
+  <si>
+    <t>FW_UI_0131</t>
+  </si>
+  <si>
+    <t>H.N,NewTest,HCVerify</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to verify RIC correction in story header for non english stories in high contrast mode.</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to verify RIC correction in alert editor for non english stories in high contrast mode.</t>
+  </si>
+  <si>
+    <t>FW_UI_0132</t>
+  </si>
+  <si>
+    <t>FW_UI_0133</t>
+  </si>
+  <si>
+    <t>H.N,Spanish,HCPublish</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to open Templates window using shortcut ket (Alt+T) in Live Feeds</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to open Templates window using shortcut ket (Alt+T) in Full Search</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to open Templates window through More Actions buttons in Live Feeds</t>
+  </si>
+  <si>
+    <t>Aim of the Script  is to open Templates window through More Actions buttons in Full Search</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to open Headline Activity window through More Actions buttons in Live Feeds</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to open Headline Activity window through More Actions buttons in Full Search</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to open Publish History window using shortcut ket (Alt+Y) in Live Feeds</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to open Publish History window using shortcut ket (Alt+Y) in Full Search</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to open More Actions dropdown using shortcut ket (Alt+R) in Live Feeds</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to open More Actions dropdown using shortcut ket (Alt+R) in Full Search</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to open Publish History window through More Actions buttons in Live Feeds</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to open Published History window through More Actions buttons in Full Search</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to open Company List dropdown using shortcut ket (Alt+L) in Live Feeds</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to open Company List dropdown using shortcut ket (Alt+L) in Full Search</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to open News Feeds dropdown using shortcut ket (Alt+F) in Live Feeds</t>
+  </si>
+  <si>
+    <t>Aim of the Script is to open News Feeds dropdown using shortcut ket (Alt+F) in Full Search</t>
+  </si>
+  <si>
+    <t>Verify_MoreActions</t>
+  </si>
+  <si>
+    <t>FW_UI_0134</t>
+  </si>
+  <si>
+    <t>FW_UI_0135</t>
+  </si>
+  <si>
+    <t>FW_UI_0136</t>
+  </si>
+  <si>
+    <t>FW_UI_0137</t>
+  </si>
+  <si>
+    <t>FW_UI_0138</t>
+  </si>
+  <si>
+    <t>FW_UI_0139</t>
+  </si>
+  <si>
+    <t>FW_UI_0140</t>
+  </si>
+  <si>
+    <t>FW_UI_0141</t>
+  </si>
+  <si>
+    <t>FW_UI_0142</t>
+  </si>
+  <si>
+    <t>FW_UI_0143</t>
+  </si>
+  <si>
+    <t>FW_UI_0144</t>
+  </si>
+  <si>
+    <t>FW_UI_0145</t>
+  </si>
+  <si>
+    <t>FW_UI_0146</t>
+  </si>
+  <si>
+    <t>FW_UI_0147</t>
+  </si>
+  <si>
+    <t>FW_UI_0148</t>
+  </si>
+  <si>
+    <t>FW_UI_0149</t>
+  </si>
+  <si>
+    <t>LIVEFEEDS,SHORTCUT,TEMPLATE</t>
+  </si>
+  <si>
+    <t>FULLSEARCH,MOREACTION,TEMPLATE</t>
+  </si>
+  <si>
+    <t>FULLSEARCH,SHORTCUT,TEMPLATE</t>
+  </si>
+  <si>
+    <t>LIVEFEEDS,MOREACTION,TEMPLATE</t>
+  </si>
+  <si>
+    <t>LIVEFEEDS,MOREACTION,HEADLINE</t>
+  </si>
+  <si>
+    <t>FULLSEARCH,MOREACTION,HEADLINE</t>
+  </si>
+  <si>
+    <t>LIVEFEEDS,SHORTCUT,PUBLISHHISTORY</t>
+  </si>
+  <si>
+    <t>LIVEFEEDS,SHORTCUT,MOREACTIONS</t>
+  </si>
+  <si>
+    <t>FULLSEARCH,SHORTCUT,MOREACTIONS</t>
+  </si>
+  <si>
+    <t>LIVEFEEDS,SHORTCUT,COMPANYLIST</t>
+  </si>
+  <si>
+    <t>FULLSEARCH,SHORTCUT,COMPANYLIST</t>
+  </si>
+  <si>
+    <t>FULLSEARCH,SHORTCUT,PUBLISHHISTORY</t>
+  </si>
+  <si>
+    <t>LIVEFEEDS,MOREACTION,PUBLISHHISTORY</t>
+  </si>
+  <si>
+    <t>FULLSEARCH,MOREACTION,PUBLISHHISTORY</t>
+  </si>
+  <si>
+    <t>LIVEFEEDS,SHORTCUT,NEWSFEED</t>
+  </si>
+  <si>
+    <t>FULLSEARCH,SHORTCUT,NEWSFEED</t>
+  </si>
+  <si>
+    <t>Verify_Topics_FullSearch</t>
+  </si>
+  <si>
+    <t>Aim of the Script  is to do Full Search with given Topic Codes</t>
+  </si>
+  <si>
+    <t>FW_UI_0150</t>
+  </si>
+  <si>
+    <t>US</t>
   </si>
 </sst>
 </file>
@@ -1356,7 +1554,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1366,6 +1564,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1458,7 +1662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1500,6 +1704,24 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1729,8 +1951,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CBB49106-BC95-4A00-9B23-0E30E5D20288}" name="Table2" displayName="Table2" ref="A1:F136" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="A1:F136" xr:uid="{CBB49106-BC95-4A00-9B23-0E30E5D20288}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CBB49106-BC95-4A00-9B23-0E30E5D20288}" name="Table2" displayName="Table2" ref="A1:F157" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:F157" xr:uid="{CBB49106-BC95-4A00-9B23-0E30E5D20288}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E8C12C75-5AB5-4A43-A3C6-442932DE8960}" name="RunTest" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{2D0C15F7-7463-4837-A664-2CE60CA101D5}" name="TC_ID" dataDxfId="4"/>
@@ -2065,10 +2287,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F136"/>
+  <dimension ref="A1:F157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C152" sqref="C152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2898,7 +3120,9 @@
       <c r="C42" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="D42" s="5"/>
+      <c r="D42" s="5" t="s">
+        <v>432</v>
+      </c>
       <c r="E42" s="7" t="s">
         <v>107</v>
       </c>
@@ -4706,7 +4930,7 @@
     </row>
     <row r="133" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B133" s="7" t="s">
         <v>425</v>
@@ -4725,39 +4949,483 @@
       </c>
     </row>
     <row r="134" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="14"/>
+      <c r="A134" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="B134" s="7" t="s">
         <v>426</v>
       </c>
-      <c r="C134" s="7"/>
-      <c r="D134" s="7"/>
-      <c r="E134" s="7"/>
+      <c r="C134" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D134" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="E134" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="F134" s="8" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="135" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="4"/>
+      <c r="A135" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="B135" s="7" t="s">
         <v>427</v>
       </c>
-      <c r="C135" s="7"/>
-      <c r="D135" s="7"/>
-      <c r="E135" s="7"/>
+      <c r="C135" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="D135" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="E135" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="F135" s="6" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="136" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="14"/>
+      <c r="A136" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="B136" s="7" t="s">
         <v>428</v>
       </c>
-      <c r="C136" s="7"/>
-      <c r="D136" s="7"/>
-      <c r="E136" s="7"/>
+      <c r="C136" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="D136" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="E136" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="F136" s="8" t="s">
         <v>413</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C137" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="D137" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="E137" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F137" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="C138" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="D138" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="E138" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F138" s="8" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="C139" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="D139" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="E139" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F139" s="6" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="C140" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="D140" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="E140" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F140" s="8" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="C141" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D141" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="E141" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F141" s="6" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="C142" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D142" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="E142" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F142" s="6" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="C143" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D143" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="E143" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F143" s="6" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B144" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="C144" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D144" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="E144" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F144" s="6" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>465</v>
+      </c>
+      <c r="C145" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D145" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="E145" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F145" s="6" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B146" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="C146" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D146" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="E146" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F146" s="6" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B147" s="7" t="s">
+        <v>467</v>
+      </c>
+      <c r="C147" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D147" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="E147" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F147" s="6" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B148" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="C148" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D148" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="E148" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F148" s="6" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B149" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="C149" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D149" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="E149" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F149" s="6" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B150" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="C150" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D150" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="E150" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F150" s="6" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B151" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="C151" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D151" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="E151" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F151" s="6" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B152" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="C152" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D152" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="E152" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F152" s="6" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B153" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="C153" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D153" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="E153" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F153" s="6" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B154" s="17" t="s">
+        <v>474</v>
+      </c>
+      <c r="C154" s="18" t="s">
+        <v>460</v>
+      </c>
+      <c r="D154" s="18" t="s">
+        <v>487</v>
+      </c>
+      <c r="E154" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="F154" s="16" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B155" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="C155" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D155" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="E155" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F155" s="6" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B156" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="C156" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D156" s="5" t="s">
+        <v>492</v>
+      </c>
+      <c r="E156" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F156" s="8" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="15" t="s">
+        <v>402</v>
+      </c>
+      <c r="B157" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="C157" s="19" t="s">
+        <v>493</v>
+      </c>
+      <c r="D157" s="19" t="s">
+        <v>496</v>
+      </c>
+      <c r="E157" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F157" s="7" t="s">
+        <v>494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Country feed snapshots and code
</commit_message>
<xml_diff>
--- a/LYNX_Automation/src/test/resources/TestData/Test_Data.xlsx
+++ b/LYNX_Automation/src/test/resources/TestData/Test_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X023840\git\Fastwire_Sikuli\LYNX_Automation\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9763EA-BC94-4589-BBA1-7F13D3107EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4074C31F-E47A-479B-9367-455CAF530005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1846" uniqueCount="954">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="951">
   <si>
     <t>RunTest</t>
   </si>
@@ -1409,9 +1409,6 @@
     <t>Aim of the Script is to open Company List dropdown using shortcut ket (Alt+L) in Live Feeds</t>
   </si>
   <si>
-    <t>Aim of the Script is to open Company List dropdown using shortcut ket (Alt+L) in Full Search</t>
-  </si>
-  <si>
     <t>Aim of the Script is to open News Feeds dropdown using shortcut ket (Alt+F) in Live Feeds</t>
   </si>
   <si>
@@ -1499,9 +1496,6 @@
     <t>LIVEFEEDS,SHORTCUT,COMPANYLIST</t>
   </si>
   <si>
-    <t>FULLSEARCH,SHORTCUT,COMPANYLIST</t>
-  </si>
-  <si>
     <t>FULLSEARCH,SHORTCUT,PUBLISHHISTORY</t>
   </si>
   <si>
@@ -2459,9 +2453,6 @@
     <t>Benelux,@Luxembourg_Web,C.N,NO</t>
   </si>
   <si>
-    <t>Benelux,@Netherlanda_Web,C.N,NO</t>
-  </si>
-  <si>
     <t>Benelux,HUGBE,C.N,NO</t>
   </si>
   <si>
@@ -2894,10 +2885,10 @@
     <t>UnitedKingdom,@ukecon,C.N,NO</t>
   </si>
   <si>
-    <t>FW_UI_0302</t>
-  </si>
-  <si>
     <t>Austria,@vienna_nr,C.N,NO</t>
+  </si>
+  <si>
+    <t>Benelux,@Netherlands_Web,C.N,NO</t>
   </si>
 </sst>
 </file>
@@ -2927,7 +2918,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2937,12 +2928,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3048,7 +3033,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -3086,19 +3071,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3331,7 +3304,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CBB49106-BC95-4A00-9B23-0E30E5D20288}" name="Table2" displayName="Table2" ref="A1:F309" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CBB49106-BC95-4A00-9B23-0E30E5D20288}" name="Table2" displayName="Table2" ref="A1:F308" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E8C12C75-5AB5-4A43-A3C6-442932DE8960}" name="RunTest" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{2D0C15F7-7463-4837-A664-2CE60CA101D5}" name="TC_ID" dataDxfId="4"/>
@@ -3666,10 +3639,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F309"/>
+  <dimension ref="A1:F308"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D182" sqref="D182"/>
+    <sheetView tabSelected="1" topLeftCell="A214" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A225" sqref="A225:A232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3713,7 +3686,7 @@
       <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="18"/>
+      <c r="D2" s="14"/>
       <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
@@ -6472,13 +6445,13 @@
         <v>30</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D141" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E141" s="7" t="s">
         <v>107</v>
@@ -6492,13 +6465,13 @@
         <v>30</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E142" s="7" t="s">
         <v>107</v>
@@ -6512,13 +6485,13 @@
         <v>30</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E143" s="7" t="s">
         <v>107</v>
@@ -6532,13 +6505,13 @@
         <v>30</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E144" s="7" t="s">
         <v>107</v>
@@ -6552,13 +6525,13 @@
         <v>30</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D145" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E145" s="7" t="s">
         <v>107</v>
@@ -6572,13 +6545,13 @@
         <v>30</v>
       </c>
       <c r="B146" s="7" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E146" s="7" t="s">
         <v>107</v>
@@ -6592,13 +6565,13 @@
         <v>30</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D147" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E147" s="7" t="s">
         <v>107</v>
@@ -6612,13 +6585,13 @@
         <v>30</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D148" s="5" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="E148" s="7" t="s">
         <v>107</v>
@@ -6632,13 +6605,13 @@
         <v>30</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D149" s="5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E149" s="7" t="s">
         <v>107</v>
@@ -6652,13 +6625,13 @@
         <v>30</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D150" s="5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E150" s="7" t="s">
         <v>107</v>
@@ -6672,13 +6645,13 @@
         <v>30</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D151" s="5" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="E151" s="7" t="s">
         <v>107</v>
@@ -6692,13 +6665,13 @@
         <v>30</v>
       </c>
       <c r="B152" s="7" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D152" s="5" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="E152" s="7" t="s">
         <v>107</v>
@@ -6712,13 +6685,13 @@
         <v>30</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D153" s="5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E153" s="7" t="s">
         <v>107</v>
@@ -6728,22 +6701,22 @@
       </c>
     </row>
     <row r="154" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B154" s="14" t="s">
-        <v>474</v>
-      </c>
-      <c r="C154" s="15" t="s">
-        <v>460</v>
-      </c>
-      <c r="D154" s="15" t="s">
-        <v>487</v>
-      </c>
-      <c r="E154" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="F154" s="13" t="s">
+      <c r="A154" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B154" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="C154" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="D154" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="E154" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F154" s="6" t="s">
         <v>457</v>
       </c>
     </row>
@@ -6752,250 +6725,250 @@
         <v>30</v>
       </c>
       <c r="B155" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="C155" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="D155" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="E155" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F155" s="8" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B156" s="7" t="s">
         <v>475</v>
       </c>
-      <c r="C155" s="5" t="s">
-        <v>460</v>
-      </c>
-      <c r="D155" s="5" t="s">
+      <c r="C156" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="E155" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="F155" s="6" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B156" s="7" t="s">
-        <v>476</v>
-      </c>
-      <c r="C156" s="5" t="s">
-        <v>460</v>
-      </c>
-      <c r="D156" s="5" t="s">
+      <c r="D156" s="13" t="s">
+        <v>494</v>
+      </c>
+      <c r="E156" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F156" s="7" t="s">
         <v>492</v>
       </c>
-      <c r="E156" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="F156" s="8" t="s">
-        <v>459</v>
-      </c>
     </row>
     <row r="157" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="12" t="s">
+      <c r="A157" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B157" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="C157" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="D157" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="E157" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F157" s="8" t="s">
         <v>495</v>
-      </c>
-      <c r="C157" s="16" t="s">
-        <v>493</v>
-      </c>
-      <c r="D157" s="16" t="s">
-        <v>496</v>
-      </c>
-      <c r="E157" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="F157" s="7" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B158" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="C158" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="D158" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="E158" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F158" s="8" t="s">
         <v>498</v>
-      </c>
-      <c r="C158" s="7" t="s">
-        <v>499</v>
-      </c>
-      <c r="D158" s="7" t="s">
-        <v>502</v>
-      </c>
-      <c r="E158" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="F158" s="8" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C159" s="7" t="s">
-        <v>499</v>
-      </c>
-      <c r="D159" s="7" t="s">
-        <v>503</v>
+        <v>497</v>
+      </c>
+      <c r="D159" s="5" t="s">
+        <v>794</v>
       </c>
       <c r="E159" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F159" s="8" t="s">
-        <v>500</v>
+      <c r="F159" s="6" t="s">
+        <v>644</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C160" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D160" s="5" t="s">
-        <v>796</v>
+        <v>949</v>
       </c>
       <c r="E160" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F160" s="6" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="161" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C161" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D161" s="5" t="s">
-        <v>953</v>
+        <v>795</v>
       </c>
       <c r="E161" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F161" s="6" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B162" s="7" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="C162" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D162" s="5" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E162" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F162" s="6" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
     </row>
     <row r="163" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B163" s="7" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C163" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D163" s="5" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E163" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F163" s="6" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="164" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B164" s="7" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="C164" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D164" s="5" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E164" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F164" s="6" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B165" s="7" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C165" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D165" s="5" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E165" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F165" s="6" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
     </row>
     <row r="166" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B166" s="7" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C166" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D166" s="5" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E166" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F166" s="6" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B167" s="7" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C167" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D167" s="5" t="s">
         <v>802</v>
@@ -7004,1307 +6977,1307 @@
         <v>107</v>
       </c>
       <c r="F167" s="6" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
     <row r="168" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B168" s="7" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="C168" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D168" s="5" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E168" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F168" s="6" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
     </row>
     <row r="169" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B169" s="7" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C169" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D169" s="5" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E169" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F169" s="6" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
     </row>
     <row r="170" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C170" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D170" s="5" t="s">
-        <v>806</v>
+        <v>950</v>
       </c>
       <c r="E170" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F170" s="6" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
     </row>
     <row r="171" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B171" s="7" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C171" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D171" s="5" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="E171" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F171" s="6" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C172" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D172" s="5" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="E172" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F172" s="6" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C173" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D173" s="5" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="E173" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F173" s="6" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B174" s="7" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C174" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D174" s="5" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="E174" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F174" s="6" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B175" s="7" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C175" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D175" s="5" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E175" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F175" s="6" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
     </row>
     <row r="176" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B176" s="7" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="C176" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D176" s="5" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="E176" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F176" s="6" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
     </row>
     <row r="177" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C177" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D177" s="5" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E177" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F177" s="6" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="178" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B178" s="7" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="C178" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D178" s="5" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
       <c r="E178" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F178" s="6" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="179" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B179" s="7" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C179" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D179" s="5" t="s">
-        <v>803</v>
+        <v>815</v>
       </c>
       <c r="E179" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F179" s="6" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="180" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B180" s="7" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="C180" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D180" s="5" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E180" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F180" s="6" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
     </row>
     <row r="181" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B181" s="7" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C181" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D181" s="5" t="s">
-        <v>820</v>
+        <v>812</v>
       </c>
       <c r="E181" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F181" s="6" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
     </row>
     <row r="182" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B182" s="7" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C182" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D182" s="5" t="s">
-        <v>815</v>
+        <v>821</v>
       </c>
       <c r="E182" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F182" s="6" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="183" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B183" s="7" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="C183" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D183" s="5" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="E183" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F183" s="6" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="184" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B184" s="7" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="C184" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D184" s="5" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="E184" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F184" s="6" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
     </row>
     <row r="185" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B185" s="7" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="C185" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D185" s="5" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="E185" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F185" s="6" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
     </row>
     <row r="186" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B186" s="7" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C186" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D186" s="5" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="E186" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F186" s="6" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B187" s="7" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="C187" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D187" s="5" t="s">
-        <v>828</v>
+        <v>816</v>
       </c>
       <c r="E187" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F187" s="6" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="188" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B188" s="7" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="C188" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D188" s="5" t="s">
-        <v>819</v>
+        <v>826</v>
       </c>
       <c r="E188" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F188" s="6" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="189" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B189" s="7" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C189" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D189" s="5" t="s">
-        <v>829</v>
+        <v>818</v>
       </c>
       <c r="E189" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F189" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="190" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B190" s="7" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="C190" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D190" s="5" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E190" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F190" s="6" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B191" s="7" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C191" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D191" s="5" t="s">
-        <v>822</v>
+        <v>813</v>
       </c>
       <c r="E191" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F191" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="192" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B192" s="7" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="C192" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D192" s="5" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="E192" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F192" s="6" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="193" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B193" s="7" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C193" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D193" s="5" t="s">
-        <v>817</v>
+        <v>820</v>
       </c>
       <c r="E193" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F193" s="6" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="194" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B194" s="7" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C194" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D194" s="5" t="s">
-        <v>823</v>
+        <v>827</v>
       </c>
       <c r="E194" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F194" s="6" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="195" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B195" s="7" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C195" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D195" s="5" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="E195" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F195" s="6" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="196" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B196" s="7" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="C196" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D196" s="5" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="E196" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F196" s="6" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="197" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B197" s="7" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C197" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D197" s="5" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="E197" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F197" s="6" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="198" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B198" s="7" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="C198" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D198" s="5" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="E198" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F198" s="6" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="199" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B199" s="7" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="C199" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D199" s="5" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="E199" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F199" s="6" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="200" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B200" s="7" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="C200" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D200" s="5" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="E200" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F200" s="6" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="201" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B201" s="7" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="C201" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D201" s="5" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="E201" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F201" s="6" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="202" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B202" s="7" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="C202" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D202" s="5" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="E202" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F202" s="6" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="203" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B203" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="C203" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D203" s="5" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="E203" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F203" s="6" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="204" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B204" s="7" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="C204" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D204" s="5" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="E204" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F204" s="6" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="205" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B205" s="7" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="C205" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D205" s="5" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="E205" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F205" s="6" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="206" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B206" s="7" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="C206" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D206" s="5" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="E206" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F206" s="6" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="207" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B207" s="7" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="C207" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D207" s="5" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="E207" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F207" s="6" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="208" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B208" s="7" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C208" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D208" s="5" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="E208" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F208" s="6" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="209" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B209" s="7" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="C209" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D209" s="5" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="E209" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F209" s="6" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="210" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B210" s="7" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C210" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D210" s="5" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="E210" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F210" s="6" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="211" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B211" s="7" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C211" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D211" s="5" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="E211" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F211" s="6" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="212" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B212" s="7" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C212" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D212" s="5" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="E212" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F212" s="6" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="213" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B213" s="7" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="C213" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D213" s="5" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="E213" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F213" s="6" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="214" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B214" s="7" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="C214" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D214" s="5" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="E214" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F214" s="6" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="215" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B215" s="7" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="C215" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D215" s="5" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="E215" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F215" s="6" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="216" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B216" s="7" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="C216" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D216" s="5" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="E216" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F216" s="6" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="217" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B217" s="7" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="C217" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D217" s="5" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="E217" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F217" s="6" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="218" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B218" s="7" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="C218" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D218" s="5" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="E218" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F218" s="6" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="219" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B219" s="7" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="C219" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D219" s="5" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="E219" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F219" s="6" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="220" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B220" s="7" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="C220" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D220" s="5" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="E220" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F220" s="6" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="221" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B221" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="C221" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D221" s="5" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="E221" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F221" s="6" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="222" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B222" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="C222" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D222" s="5" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="E222" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F222" s="6" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="223" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B223" s="7" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="C223" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D223" s="5" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="E223" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F223" s="6" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="224" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B224" s="7" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="C224" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D224" s="5" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="E224" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F224" s="6" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="225" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B225" s="7" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="C225" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D225" s="5" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="E225" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F225" s="6" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="226" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B226" s="7" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C226" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D226" s="5" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="E226" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F226" s="6" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="227" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B227" s="7" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="C227" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D227" s="5" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="E227" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F227" s="6" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="228" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B228" s="7" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="C228" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D228" s="5" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="E228" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F228" s="6" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="229" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B229" s="7" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="C229" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D229" s="5" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="E229" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F229" s="6" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="230" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B230" s="7" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="C230" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D230" s="5" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="E230" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F230" s="6" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="231" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B231" s="7" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="C231" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D231" s="5" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="E231" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F231" s="6" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="232" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="11" t="s">
-        <v>402</v>
+        <v>30</v>
       </c>
       <c r="B232" s="7" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="C232" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D232" s="5" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="E232" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F232" s="6" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="233" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8312,19 +8285,19 @@
         <v>402</v>
       </c>
       <c r="B233" s="7" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="C233" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D233" s="5" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="E233" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F233" s="6" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="234" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8332,19 +8305,19 @@
         <v>402</v>
       </c>
       <c r="B234" s="7" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="C234" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D234" s="5" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="E234" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F234" s="6" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="235" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8352,19 +8325,19 @@
         <v>402</v>
       </c>
       <c r="B235" s="7" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="C235" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D235" s="5" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="E235" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F235" s="6" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
     </row>
     <row r="236" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8372,19 +8345,19 @@
         <v>402</v>
       </c>
       <c r="B236" s="7" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="C236" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D236" s="5" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="E236" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F236" s="6" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="237" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8392,19 +8365,19 @@
         <v>402</v>
       </c>
       <c r="B237" s="7" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="C237" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D237" s="5" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="E237" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F237" s="6" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="238" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8412,19 +8385,19 @@
         <v>402</v>
       </c>
       <c r="B238" s="7" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="C238" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D238" s="5" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="E238" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F238" s="6" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="239" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8432,19 +8405,19 @@
         <v>402</v>
       </c>
       <c r="B239" s="7" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="C239" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D239" s="5" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="E239" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F239" s="6" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="240" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8452,19 +8425,19 @@
         <v>402</v>
       </c>
       <c r="B240" s="7" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="C240" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D240" s="5" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="E240" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F240" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="241" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8472,19 +8445,19 @@
         <v>402</v>
       </c>
       <c r="B241" s="7" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="C241" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D241" s="5" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="E241" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F241" s="6" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="242" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8492,19 +8465,19 @@
         <v>402</v>
       </c>
       <c r="B242" s="7" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="C242" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D242" s="5" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="E242" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F242" s="6" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="243" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8512,19 +8485,19 @@
         <v>402</v>
       </c>
       <c r="B243" s="7" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="C243" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D243" s="5" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="E243" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F243" s="6" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="244" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8532,19 +8505,19 @@
         <v>402</v>
       </c>
       <c r="B244" s="7" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="C244" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D244" s="5" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="E244" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F244" s="6" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="245" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8552,19 +8525,19 @@
         <v>402</v>
       </c>
       <c r="B245" s="7" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="C245" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D245" s="5" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="E245" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F245" s="6" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="246" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8572,19 +8545,19 @@
         <v>402</v>
       </c>
       <c r="B246" s="7" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="C246" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D246" s="5" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="E246" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F246" s="6" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="247" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8592,19 +8565,19 @@
         <v>402</v>
       </c>
       <c r="B247" s="7" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="C247" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D247" s="5" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="E247" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F247" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="248" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8612,19 +8585,19 @@
         <v>402</v>
       </c>
       <c r="B248" s="7" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="C248" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D248" s="5" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="E248" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F248" s="6" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="249" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8632,19 +8605,19 @@
         <v>402</v>
       </c>
       <c r="B249" s="7" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="C249" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D249" s="5" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="E249" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F249" s="6" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="250" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8652,19 +8625,19 @@
         <v>402</v>
       </c>
       <c r="B250" s="7" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="C250" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D250" s="5" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="E250" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F250" s="6" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="251" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8672,19 +8645,19 @@
         <v>402</v>
       </c>
       <c r="B251" s="7" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="C251" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D251" s="5" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="E251" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F251" s="6" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="252" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8692,19 +8665,19 @@
         <v>402</v>
       </c>
       <c r="B252" s="7" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C252" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D252" s="5" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="E252" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F252" s="6" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="253" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8712,19 +8685,19 @@
         <v>402</v>
       </c>
       <c r="B253" s="7" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C253" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D253" s="5" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="E253" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F253" s="6" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="254" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8732,19 +8705,19 @@
         <v>402</v>
       </c>
       <c r="B254" s="7" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="C254" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D254" s="5" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="E254" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F254" s="6" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="255" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8752,19 +8725,19 @@
         <v>402</v>
       </c>
       <c r="B255" s="7" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="C255" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D255" s="5" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="E255" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F255" s="6" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="256" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8772,19 +8745,19 @@
         <v>402</v>
       </c>
       <c r="B256" s="7" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C256" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D256" s="5" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="E256" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F256" s="6" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="257" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8792,19 +8765,19 @@
         <v>402</v>
       </c>
       <c r="B257" s="7" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="C257" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D257" s="5" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="E257" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F257" s="6" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="258" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8812,19 +8785,19 @@
         <v>402</v>
       </c>
       <c r="B258" s="7" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C258" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D258" s="5" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="E258" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F258" s="6" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="259" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8832,19 +8805,19 @@
         <v>402</v>
       </c>
       <c r="B259" s="7" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="C259" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D259" s="5" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="E259" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F259" s="6" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="260" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8852,19 +8825,19 @@
         <v>402</v>
       </c>
       <c r="B260" s="7" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="C260" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D260" s="5" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="E260" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F260" s="6" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="261" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8872,19 +8845,19 @@
         <v>402</v>
       </c>
       <c r="B261" s="7" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C261" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D261" s="5" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="E261" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F261" s="6" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="262" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8892,19 +8865,19 @@
         <v>402</v>
       </c>
       <c r="B262" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="C262" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D262" s="5" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="E262" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F262" s="6" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="263" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8912,19 +8885,19 @@
         <v>402</v>
       </c>
       <c r="B263" s="7" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="C263" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D263" s="5" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="E263" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F263" s="6" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="264" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8932,19 +8905,19 @@
         <v>402</v>
       </c>
       <c r="B264" s="7" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C264" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D264" s="5" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="E264" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F264" s="6" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="265" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8952,19 +8925,19 @@
         <v>402</v>
       </c>
       <c r="B265" s="7" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="C265" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D265" s="5" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="E265" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F265" s="6" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="266" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8972,19 +8945,19 @@
         <v>402</v>
       </c>
       <c r="B266" s="7" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="C266" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D266" s="5" t="s">
-        <v>901</v>
+        <v>931</v>
       </c>
       <c r="E266" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F266" s="6" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="267" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8992,19 +8965,19 @@
         <v>402</v>
       </c>
       <c r="B267" s="7" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="C267" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D267" s="5" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="E267" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F267" s="6" t="s">
-        <v>539</v>
+        <v>933</v>
       </c>
     </row>
     <row r="268" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9012,19 +8985,19 @@
         <v>402</v>
       </c>
       <c r="B268" s="7" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="C268" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D268" s="5" t="s">
-        <v>935</v>
+        <v>899</v>
       </c>
       <c r="E268" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F268" s="6" t="s">
-        <v>936</v>
+        <v>536</v>
       </c>
     </row>
     <row r="269" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9032,19 +9005,19 @@
         <v>402</v>
       </c>
       <c r="B269" s="7" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="C269" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D269" s="5" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="E269" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F269" s="6" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="270" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9052,19 +9025,19 @@
         <v>402</v>
       </c>
       <c r="B270" s="7" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="C270" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D270" s="5" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="E270" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F270" s="6" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="271" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9072,19 +9045,19 @@
         <v>402</v>
       </c>
       <c r="B271" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="C271" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D271" s="5" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="E271" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F271" s="6" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="272" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9092,19 +9065,19 @@
         <v>402</v>
       </c>
       <c r="B272" s="7" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C272" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D272" s="5" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="E272" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F272" s="6" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="273" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9112,19 +9085,19 @@
         <v>402</v>
       </c>
       <c r="B273" s="7" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="C273" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D273" s="5" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="E273" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F273" s="6" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="274" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9132,19 +9105,19 @@
         <v>402</v>
       </c>
       <c r="B274" s="7" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="C274" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D274" s="5" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="E274" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F274" s="6" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="275" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9152,19 +9125,19 @@
         <v>402</v>
       </c>
       <c r="B275" s="7" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="C275" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D275" s="5" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="E275" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F275" s="6" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="276" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9172,19 +9145,19 @@
         <v>402</v>
       </c>
       <c r="B276" s="7" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="C276" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D276" s="5" t="s">
-        <v>909</v>
+        <v>934</v>
       </c>
       <c r="E276" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F276" s="6" t="s">
-        <v>531</v>
+        <v>938</v>
       </c>
     </row>
     <row r="277" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9192,13 +9165,13 @@
         <v>402</v>
       </c>
       <c r="B277" s="7" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="C277" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D277" s="5" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="E277" s="7" t="s">
         <v>107</v>
@@ -9212,19 +9185,19 @@
         <v>402</v>
       </c>
       <c r="B278" s="7" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="C278" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D278" s="5" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="E278" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F278" s="6" t="s">
-        <v>944</v>
+        <v>939</v>
       </c>
     </row>
     <row r="279" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9232,19 +9205,19 @@
         <v>402</v>
       </c>
       <c r="B279" s="7" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="C279" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D279" s="5" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="E279" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F279" s="6" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
     </row>
     <row r="280" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9252,19 +9225,19 @@
         <v>402</v>
       </c>
       <c r="B280" s="7" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C280" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D280" s="5" t="s">
-        <v>940</v>
+        <v>907</v>
       </c>
       <c r="E280" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F280" s="6" t="s">
-        <v>943</v>
+        <v>528</v>
       </c>
     </row>
     <row r="281" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9272,19 +9245,19 @@
         <v>402</v>
       </c>
       <c r="B281" s="7" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="C281" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D281" s="5" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="E281" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F281" s="6" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="282" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9292,19 +9265,19 @@
         <v>402</v>
       </c>
       <c r="B282" s="7" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C282" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D282" s="5" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="E282" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F282" s="6" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="283" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9312,19 +9285,19 @@
         <v>402</v>
       </c>
       <c r="B283" s="7" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="C283" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D283" s="5" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="E283" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F283" s="6" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="284" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9332,19 +9305,19 @@
         <v>402</v>
       </c>
       <c r="B284" s="7" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C284" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D284" s="5" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="E284" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F284" s="6" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="285" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9352,19 +9325,19 @@
         <v>402</v>
       </c>
       <c r="B285" s="7" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="C285" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D285" s="5" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="E285" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F285" s="6" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="286" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9372,19 +9345,19 @@
         <v>402</v>
       </c>
       <c r="B286" s="7" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="C286" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D286" s="5" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="E286" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F286" s="6" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="287" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9392,19 +9365,19 @@
         <v>402</v>
       </c>
       <c r="B287" s="7" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C287" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D287" s="5" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="E287" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F287" s="6" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="288" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9412,19 +9385,19 @@
         <v>402</v>
       </c>
       <c r="B288" s="7" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C288" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D288" s="5" t="s">
-        <v>917</v>
+        <v>948</v>
       </c>
       <c r="E288" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F288" s="6" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="289" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9432,19 +9405,19 @@
         <v>402</v>
       </c>
       <c r="B289" s="7" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="C289" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D289" s="5" t="s">
-        <v>951</v>
+        <v>915</v>
       </c>
       <c r="E289" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F289" s="6" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="290" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9452,19 +9425,19 @@
         <v>402</v>
       </c>
       <c r="B290" s="7" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="C290" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D290" s="5" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="E290" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F290" s="6" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="291" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9472,19 +9445,19 @@
         <v>402</v>
       </c>
       <c r="B291" s="7" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="C291" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D291" s="5" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="E291" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F291" s="6" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="292" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9492,19 +9465,19 @@
         <v>402</v>
       </c>
       <c r="B292" s="7" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="C292" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D292" s="5" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="E292" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F292" s="6" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="293" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9512,19 +9485,19 @@
         <v>402</v>
       </c>
       <c r="B293" s="7" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="C293" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D293" s="5" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="E293" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F293" s="6" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="294" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9532,19 +9505,19 @@
         <v>402</v>
       </c>
       <c r="B294" s="7" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C294" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D294" s="5" t="s">
-        <v>922</v>
+        <v>946</v>
       </c>
       <c r="E294" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F294" s="6" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="295" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9552,19 +9525,19 @@
         <v>402</v>
       </c>
       <c r="B295" s="7" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C295" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D295" s="5" t="s">
-        <v>949</v>
+        <v>920</v>
       </c>
       <c r="E295" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F295" s="6" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="296" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9572,19 +9545,19 @@
         <v>402</v>
       </c>
       <c r="B296" s="7" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C296" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D296" s="5" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="E296" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F296" s="6" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="297" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9592,19 +9565,19 @@
         <v>402</v>
       </c>
       <c r="B297" s="7" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C297" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D297" s="5" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="E297" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F297" s="6" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="298" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9612,19 +9585,19 @@
         <v>402</v>
       </c>
       <c r="B298" s="7" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C298" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D298" s="5" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="E298" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F298" s="6" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="299" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9632,19 +9605,19 @@
         <v>402</v>
       </c>
       <c r="B299" s="7" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="C299" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D299" s="5" t="s">
-        <v>926</v>
+        <v>947</v>
       </c>
       <c r="E299" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F299" s="6" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="300" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9652,19 +9625,19 @@
         <v>402</v>
       </c>
       <c r="B300" s="7" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="C300" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D300" s="5" t="s">
-        <v>950</v>
+        <v>924</v>
       </c>
       <c r="E300" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F300" s="6" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="301" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9672,19 +9645,19 @@
         <v>402</v>
       </c>
       <c r="B301" s="7" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="C301" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D301" s="5" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="E301" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F301" s="6" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="302" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9692,19 +9665,19 @@
         <v>402</v>
       </c>
       <c r="B302" s="7" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="C302" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D302" s="5" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="E302" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F302" s="6" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="303" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9712,19 +9685,19 @@
         <v>402</v>
       </c>
       <c r="B303" s="7" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C303" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D303" s="5" t="s">
-        <v>929</v>
+        <v>944</v>
       </c>
       <c r="E303" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F303" s="6" t="s">
-        <v>508</v>
+        <v>942</v>
       </c>
     </row>
     <row r="304" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9732,19 +9705,19 @@
         <v>402</v>
       </c>
       <c r="B304" s="7" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C304" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D304" s="5" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="E304" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F304" s="6" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="305" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9752,19 +9725,19 @@
         <v>402</v>
       </c>
       <c r="B305" s="7" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="C305" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D305" s="5" t="s">
-        <v>948</v>
+        <v>927</v>
       </c>
       <c r="E305" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F305" s="6" t="s">
-        <v>946</v>
+        <v>505</v>
       </c>
     </row>
     <row r="306" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9772,19 +9745,19 @@
         <v>402</v>
       </c>
       <c r="B306" s="7" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="C306" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D306" s="5" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="E306" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F306" s="6" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="307" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9792,19 +9765,19 @@
         <v>402</v>
       </c>
       <c r="B307" s="7" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C307" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D307" s="5" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="E307" s="7" t="s">
         <v>107</v>
       </c>
       <c r="F307" s="6" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="308" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -9812,39 +9785,19 @@
         <v>402</v>
       </c>
       <c r="B308" s="7" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="C308" s="7" t="s">
-        <v>499</v>
-      </c>
-      <c r="D308" s="5" t="s">
-        <v>932</v>
+        <v>497</v>
+      </c>
+      <c r="D308" s="7" t="s">
+        <v>930</v>
       </c>
       <c r="E308" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F308" s="6" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="309" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A309" s="11" t="s">
-        <v>402</v>
-      </c>
-      <c r="B309" s="7" t="s">
-        <v>952</v>
-      </c>
-      <c r="C309" s="7" t="s">
-        <v>499</v>
-      </c>
-      <c r="D309" s="7" t="s">
-        <v>933</v>
-      </c>
-      <c r="E309" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="F309" s="8" t="s">
-        <v>504</v>
+      <c r="F308" s="8" t="s">
+        <v>502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit on 19 sep
</commit_message>
<xml_diff>
--- a/LYNX_Automation/src/test/resources/TestData/Test_Data.xlsx
+++ b/LYNX_Automation/src/test/resources/TestData/Test_Data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X023840\git\Fastwire_Sikuli\LYNX_Automation\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67965130-6068-44F0-80CD-5A8E419DDDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E1C208-0446-46A3-99B4-1057C6E3076E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Cases'!#REF!</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7472" uniqueCount="3677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7917" uniqueCount="3676">
   <si>
     <t>RunTest</t>
   </si>
@@ -11066,9 +11067,6 @@
   </si>
   <si>
     <t>Aim of the Script is to verify Whether selected company list, automations filters and web watchers retained in next session when user relaunches fastwire</t>
-  </si>
-  <si>
-    <t>VerifyWWScenarios</t>
   </si>
 </sst>
 </file>
@@ -11823,8 +11821,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F1309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F10" activeCellId="1" sqref="F19 F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28006,9 +28004,15 @@
       <c r="B809" s="4" t="s">
         <v>2898</v>
       </c>
-      <c r="C809" s="11"/>
-      <c r="D809" s="4"/>
-      <c r="E809" s="12"/>
+      <c r="C809" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D809" s="4" t="s">
+        <v>2108</v>
+      </c>
+      <c r="E809" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F809" s="4" t="s">
         <v>2433</v>
       </c>
@@ -28020,9 +28024,15 @@
       <c r="B810" s="4" t="s">
         <v>2899</v>
       </c>
-      <c r="C810" s="11"/>
-      <c r="D810" s="4"/>
-      <c r="E810" s="12"/>
+      <c r="C810" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D810" s="4" t="s">
+        <v>2082</v>
+      </c>
+      <c r="E810" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F810" s="4" t="s">
         <v>2434</v>
       </c>
@@ -28034,9 +28044,15 @@
       <c r="B811" s="4" t="s">
         <v>2900</v>
       </c>
-      <c r="C811" s="11"/>
-      <c r="D811" s="4"/>
-      <c r="E811" s="12"/>
+      <c r="C811" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D811" s="4" t="s">
+        <v>2109</v>
+      </c>
+      <c r="E811" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F811" s="4" t="s">
         <v>2435</v>
       </c>
@@ -28048,9 +28064,15 @@
       <c r="B812" s="4" t="s">
         <v>2901</v>
       </c>
-      <c r="C812" s="11"/>
-      <c r="D812" s="4"/>
-      <c r="E812" s="12"/>
+      <c r="C812" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D812" s="4" t="s">
+        <v>2083</v>
+      </c>
+      <c r="E812" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F812" s="4" t="s">
         <v>2436</v>
       </c>
@@ -28062,9 +28084,15 @@
       <c r="B813" s="4" t="s">
         <v>2902</v>
       </c>
-      <c r="C813" s="11"/>
-      <c r="D813" s="4"/>
-      <c r="E813" s="12"/>
+      <c r="C813" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D813" s="4" t="s">
+        <v>2110</v>
+      </c>
+      <c r="E813" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F813" s="4" t="s">
         <v>2437</v>
       </c>
@@ -28076,9 +28104,15 @@
       <c r="B814" s="4" t="s">
         <v>2903</v>
       </c>
-      <c r="C814" s="11"/>
-      <c r="D814" s="4"/>
-      <c r="E814" s="12"/>
+      <c r="C814" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D814" s="4" t="s">
+        <v>2084</v>
+      </c>
+      <c r="E814" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F814" s="4" t="s">
         <v>2438</v>
       </c>
@@ -28090,9 +28124,15 @@
       <c r="B815" s="4" t="s">
         <v>2904</v>
       </c>
-      <c r="C815" s="11"/>
-      <c r="D815" s="4"/>
-      <c r="E815" s="12"/>
+      <c r="C815" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D815" s="4" t="s">
+        <v>2111</v>
+      </c>
+      <c r="E815" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F815" s="4" t="s">
         <v>2439</v>
       </c>
@@ -28104,9 +28144,15 @@
       <c r="B816" s="4" t="s">
         <v>2905</v>
       </c>
-      <c r="C816" s="11"/>
-      <c r="D816" s="4"/>
-      <c r="E816" s="12"/>
+      <c r="C816" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D816" s="4" t="s">
+        <v>2085</v>
+      </c>
+      <c r="E816" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F816" s="4" t="s">
         <v>2440</v>
       </c>
@@ -28118,9 +28164,15 @@
       <c r="B817" s="4" t="s">
         <v>2906</v>
       </c>
-      <c r="C817" s="11"/>
-      <c r="D817" s="4"/>
-      <c r="E817" s="12"/>
+      <c r="C817" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D817" s="4" t="s">
+        <v>2112</v>
+      </c>
+      <c r="E817" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F817" s="4" t="s">
         <v>2441</v>
       </c>
@@ -28132,9 +28184,15 @@
       <c r="B818" s="4" t="s">
         <v>2907</v>
       </c>
-      <c r="C818" s="11"/>
-      <c r="D818" s="4"/>
-      <c r="E818" s="12"/>
+      <c r="C818" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D818" s="4" t="s">
+        <v>2086</v>
+      </c>
+      <c r="E818" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F818" s="4" t="s">
         <v>2442</v>
       </c>
@@ -28146,9 +28204,15 @@
       <c r="B819" s="4" t="s">
         <v>2908</v>
       </c>
-      <c r="C819" s="11"/>
-      <c r="D819" s="4"/>
-      <c r="E819" s="12"/>
+      <c r="C819" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D819" s="4" t="s">
+        <v>2113</v>
+      </c>
+      <c r="E819" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F819" s="4" t="s">
         <v>2443</v>
       </c>
@@ -28160,9 +28224,15 @@
       <c r="B820" s="4" t="s">
         <v>2909</v>
       </c>
-      <c r="C820" s="11"/>
-      <c r="D820" s="4"/>
-      <c r="E820" s="12"/>
+      <c r="C820" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D820" s="4" t="s">
+        <v>2087</v>
+      </c>
+      <c r="E820" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F820" s="4" t="s">
         <v>2444</v>
       </c>
@@ -28174,9 +28244,15 @@
       <c r="B821" s="4" t="s">
         <v>2910</v>
       </c>
-      <c r="C821" s="11"/>
-      <c r="D821" s="4"/>
-      <c r="E821" s="12"/>
+      <c r="C821" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D821" s="4" t="s">
+        <v>2114</v>
+      </c>
+      <c r="E821" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F821" s="4" t="s">
         <v>2445</v>
       </c>
@@ -28188,9 +28264,15 @@
       <c r="B822" s="4" t="s">
         <v>2911</v>
       </c>
-      <c r="C822" s="11"/>
-      <c r="D822" s="4"/>
-      <c r="E822" s="12"/>
+      <c r="C822" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D822" s="4" t="s">
+        <v>2088</v>
+      </c>
+      <c r="E822" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F822" s="4" t="s">
         <v>2446</v>
       </c>
@@ -28202,9 +28284,15 @@
       <c r="B823" s="4" t="s">
         <v>2912</v>
       </c>
-      <c r="C823" s="11"/>
-      <c r="D823" s="4"/>
-      <c r="E823" s="12"/>
+      <c r="C823" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D823" s="4" t="s">
+        <v>2115</v>
+      </c>
+      <c r="E823" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F823" s="4" t="s">
         <v>2447</v>
       </c>
@@ -28216,9 +28304,15 @@
       <c r="B824" s="4" t="s">
         <v>2913</v>
       </c>
-      <c r="C824" s="11"/>
-      <c r="D824" s="4"/>
-      <c r="E824" s="12"/>
+      <c r="C824" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D824" s="4" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E824" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F824" s="4" t="s">
         <v>2448</v>
       </c>
@@ -28230,9 +28324,15 @@
       <c r="B825" s="4" t="s">
         <v>2914</v>
       </c>
-      <c r="C825" s="11"/>
-      <c r="D825" s="4"/>
-      <c r="E825" s="12"/>
+      <c r="C825" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D825" s="4" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E825" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F825" s="4" t="s">
         <v>2449</v>
       </c>
@@ -28244,9 +28344,15 @@
       <c r="B826" s="4" t="s">
         <v>2915</v>
       </c>
-      <c r="C826" s="11"/>
-      <c r="D826" s="4"/>
-      <c r="E826" s="12"/>
+      <c r="C826" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D826" s="4" t="s">
+        <v>2090</v>
+      </c>
+      <c r="E826" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F826" s="4" t="s">
         <v>2450</v>
       </c>
@@ -28258,9 +28364,15 @@
       <c r="B827" s="4" t="s">
         <v>2916</v>
       </c>
-      <c r="C827" s="11"/>
-      <c r="D827" s="4"/>
-      <c r="E827" s="12"/>
+      <c r="C827" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D827" s="4" t="s">
+        <v>2091</v>
+      </c>
+      <c r="E827" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F827" s="4" t="s">
         <v>2451</v>
       </c>
@@ -28272,9 +28384,15 @@
       <c r="B828" s="4" t="s">
         <v>2917</v>
       </c>
-      <c r="C828" s="11"/>
-      <c r="D828" s="4"/>
-      <c r="E828" s="12"/>
+      <c r="C828" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D828" s="4" t="s">
+        <v>2092</v>
+      </c>
+      <c r="E828" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F828" s="4" t="s">
         <v>2452</v>
       </c>
@@ -28286,9 +28404,15 @@
       <c r="B829" s="4" t="s">
         <v>2918</v>
       </c>
-      <c r="C829" s="11"/>
-      <c r="D829" s="4"/>
-      <c r="E829" s="12"/>
+      <c r="C829" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D829" s="4" t="s">
+        <v>2093</v>
+      </c>
+      <c r="E829" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F829" s="4" t="s">
         <v>2453</v>
       </c>
@@ -28300,9 +28424,15 @@
       <c r="B830" s="4" t="s">
         <v>2919</v>
       </c>
-      <c r="C830" s="11"/>
-      <c r="D830" s="4"/>
-      <c r="E830" s="12"/>
+      <c r="C830" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D830" s="4" t="s">
+        <v>2094</v>
+      </c>
+      <c r="E830" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F830" s="4" t="s">
         <v>2454</v>
       </c>
@@ -28314,9 +28444,15 @@
       <c r="B831" s="4" t="s">
         <v>2920</v>
       </c>
-      <c r="C831" s="11"/>
-      <c r="D831" s="4"/>
-      <c r="E831" s="12"/>
+      <c r="C831" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="D831" s="4" t="s">
+        <v>949</v>
+      </c>
+      <c r="E831" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F831" s="4" t="s">
         <v>2455</v>
       </c>
@@ -28328,9 +28464,15 @@
       <c r="B832" s="4" t="s">
         <v>2921</v>
       </c>
-      <c r="C832" s="11"/>
-      <c r="D832" s="4"/>
-      <c r="E832" s="12"/>
+      <c r="C832" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="D832" s="4" t="s">
+        <v>950</v>
+      </c>
+      <c r="E832" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F832" s="4" t="s">
         <v>2456</v>
       </c>
@@ -28342,9 +28484,15 @@
       <c r="B833" s="4" t="s">
         <v>2922</v>
       </c>
-      <c r="C833" s="11"/>
-      <c r="D833" s="4"/>
-      <c r="E833" s="12"/>
+      <c r="C833" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="D833" s="4" t="s">
+        <v>951</v>
+      </c>
+      <c r="E833" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F833" s="4" t="s">
         <v>2457</v>
       </c>
@@ -28356,9 +28504,15 @@
       <c r="B834" s="4" t="s">
         <v>2923</v>
       </c>
-      <c r="C834" s="11"/>
-      <c r="D834" s="4"/>
-      <c r="E834" s="12"/>
+      <c r="C834" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="D834" s="4" t="s">
+        <v>952</v>
+      </c>
+      <c r="E834" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F834" s="4" t="s">
         <v>2458</v>
       </c>
@@ -28370,9 +28524,15 @@
       <c r="B835" s="4" t="s">
         <v>2924</v>
       </c>
-      <c r="C835" s="11"/>
-      <c r="D835" s="4"/>
-      <c r="E835" s="12"/>
+      <c r="C835" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="D835" s="4" t="s">
+        <v>957</v>
+      </c>
+      <c r="E835" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F835" s="4" t="s">
         <v>2459</v>
       </c>
@@ -28384,9 +28544,15 @@
       <c r="B836" s="4" t="s">
         <v>2925</v>
       </c>
-      <c r="C836" s="11"/>
-      <c r="D836" s="4"/>
-      <c r="E836" s="12"/>
+      <c r="C836" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="D836" s="4" t="s">
+        <v>958</v>
+      </c>
+      <c r="E836" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F836" s="4" t="s">
         <v>2460</v>
       </c>
@@ -28398,9 +28564,15 @@
       <c r="B837" s="4" t="s">
         <v>2926</v>
       </c>
-      <c r="C837" s="11"/>
-      <c r="D837" s="4"/>
-      <c r="E837" s="12"/>
+      <c r="C837" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="D837" s="4" t="s">
+        <v>959</v>
+      </c>
+      <c r="E837" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F837" s="4" t="s">
         <v>2461</v>
       </c>
@@ -28412,9 +28584,15 @@
       <c r="B838" s="4" t="s">
         <v>2927</v>
       </c>
-      <c r="C838" s="11"/>
-      <c r="D838" s="4"/>
-      <c r="E838" s="12"/>
+      <c r="C838" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="D838" s="4" t="s">
+        <v>960</v>
+      </c>
+      <c r="E838" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F838" s="4" t="s">
         <v>2462</v>
       </c>
@@ -28426,9 +28604,15 @@
       <c r="B839" s="4" t="s">
         <v>2928</v>
       </c>
-      <c r="C839" s="11"/>
-      <c r="D839" s="4"/>
-      <c r="E839" s="12"/>
+      <c r="C839" s="4" t="s">
+        <v>962</v>
+      </c>
+      <c r="D839" s="4" t="s">
+        <v>973</v>
+      </c>
+      <c r="E839" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F839" s="4" t="s">
         <v>2463</v>
       </c>
@@ -28440,9 +28624,15 @@
       <c r="B840" s="4" t="s">
         <v>2929</v>
       </c>
-      <c r="C840" s="11"/>
-      <c r="D840" s="4"/>
-      <c r="E840" s="12"/>
+      <c r="C840" s="4" t="s">
+        <v>962</v>
+      </c>
+      <c r="D840" s="4" t="s">
+        <v>970</v>
+      </c>
+      <c r="E840" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F840" s="4" t="s">
         <v>2464</v>
       </c>
@@ -28454,9 +28644,15 @@
       <c r="B841" s="4" t="s">
         <v>2930</v>
       </c>
-      <c r="C841" s="11"/>
-      <c r="D841" s="4"/>
-      <c r="E841" s="12"/>
+      <c r="C841" s="4" t="s">
+        <v>962</v>
+      </c>
+      <c r="D841" s="4" t="s">
+        <v>971</v>
+      </c>
+      <c r="E841" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F841" s="4" t="s">
         <v>2465</v>
       </c>
@@ -28468,9 +28664,15 @@
       <c r="B842" s="4" t="s">
         <v>2931</v>
       </c>
-      <c r="C842" s="11"/>
-      <c r="D842" s="4"/>
-      <c r="E842" s="12"/>
+      <c r="C842" s="4" t="s">
+        <v>962</v>
+      </c>
+      <c r="D842" s="4" t="s">
+        <v>972</v>
+      </c>
+      <c r="E842" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F842" s="4" t="s">
         <v>2466</v>
       </c>
@@ -28482,9 +28684,15 @@
       <c r="B843" s="4" t="s">
         <v>2932</v>
       </c>
-      <c r="C843" s="11"/>
-      <c r="D843" s="4"/>
-      <c r="E843" s="12"/>
+      <c r="C843" s="4" t="s">
+        <v>985</v>
+      </c>
+      <c r="D843" s="4" t="s">
+        <v>987</v>
+      </c>
+      <c r="E843" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F843" s="4" t="s">
         <v>2467</v>
       </c>
@@ -28496,9 +28704,15 @@
       <c r="B844" s="4" t="s">
         <v>2933</v>
       </c>
-      <c r="C844" s="11"/>
-      <c r="D844" s="4"/>
-      <c r="E844" s="12"/>
+      <c r="C844" s="4" t="s">
+        <v>985</v>
+      </c>
+      <c r="D844" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="E844" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F844" s="4" t="s">
         <v>2468</v>
       </c>
@@ -28510,9 +28724,15 @@
       <c r="B845" s="4" t="s">
         <v>2934</v>
       </c>
-      <c r="C845" s="11"/>
-      <c r="D845" s="4"/>
-      <c r="E845" s="12"/>
+      <c r="C845" s="4" t="s">
+        <v>985</v>
+      </c>
+      <c r="D845" s="4" t="s">
+        <v>979</v>
+      </c>
+      <c r="E845" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F845" s="4" t="s">
         <v>2469</v>
       </c>
@@ -28524,9 +28744,15 @@
       <c r="B846" s="4" t="s">
         <v>2935</v>
       </c>
-      <c r="C846" s="11"/>
-      <c r="D846" s="4"/>
-      <c r="E846" s="12"/>
+      <c r="C846" s="4" t="s">
+        <v>985</v>
+      </c>
+      <c r="D846" s="4" t="s">
+        <v>980</v>
+      </c>
+      <c r="E846" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F846" s="4" t="s">
         <v>2470</v>
       </c>
@@ -28538,9 +28764,15 @@
       <c r="B847" s="4" t="s">
         <v>2936</v>
       </c>
-      <c r="C847" s="11"/>
-      <c r="D847" s="4"/>
-      <c r="E847" s="12"/>
+      <c r="C847" s="4" t="s">
+        <v>994</v>
+      </c>
+      <c r="D847" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="E847" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F847" s="4" t="s">
         <v>2471</v>
       </c>
@@ -28552,9 +28784,15 @@
       <c r="B848" s="4" t="s">
         <v>2937</v>
       </c>
-      <c r="C848" s="11"/>
-      <c r="D848" s="4"/>
-      <c r="E848" s="12"/>
+      <c r="C848" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D848" s="4" t="s">
+        <v>2117</v>
+      </c>
+      <c r="E848" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F848" s="4" t="s">
         <v>2472</v>
       </c>
@@ -28566,9 +28804,15 @@
       <c r="B849" s="4" t="s">
         <v>2938</v>
       </c>
-      <c r="C849" s="11"/>
-      <c r="D849" s="4"/>
-      <c r="E849" s="12"/>
+      <c r="C849" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D849" s="4" t="s">
+        <v>2095</v>
+      </c>
+      <c r="E849" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F849" s="4" t="s">
         <v>2473</v>
       </c>
@@ -28580,9 +28824,15 @@
       <c r="B850" s="4" t="s">
         <v>2939</v>
       </c>
-      <c r="C850" s="11"/>
-      <c r="D850" s="4"/>
-      <c r="E850" s="12"/>
+      <c r="C850" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="D850" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E850" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F850" s="4" t="s">
         <v>2474</v>
       </c>
@@ -28594,9 +28844,15 @@
       <c r="B851" s="4" t="s">
         <v>2940</v>
       </c>
-      <c r="C851" s="11"/>
-      <c r="D851" s="4"/>
-      <c r="E851" s="12"/>
+      <c r="C851" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="D851" s="4" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E851" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F851" s="4" t="s">
         <v>2475</v>
       </c>
@@ -28608,9 +28864,15 @@
       <c r="B852" s="4" t="s">
         <v>2941</v>
       </c>
-      <c r="C852" s="11"/>
-      <c r="D852" s="4"/>
-      <c r="E852" s="12"/>
+      <c r="C852" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="D852" s="4" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E852" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F852" s="4" t="s">
         <v>2476</v>
       </c>
@@ -28622,9 +28884,15 @@
       <c r="B853" s="4" t="s">
         <v>2942</v>
       </c>
-      <c r="C853" s="11"/>
-      <c r="D853" s="4"/>
-      <c r="E853" s="12"/>
+      <c r="C853" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="D853" s="4" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E853" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F853" s="4" t="s">
         <v>2477</v>
       </c>
@@ -28636,9 +28904,15 @@
       <c r="B854" s="4" t="s">
         <v>2943</v>
       </c>
-      <c r="C854" s="11"/>
-      <c r="D854" s="4"/>
-      <c r="E854" s="12"/>
+      <c r="C854" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="D854" s="4" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E854" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F854" s="4" t="s">
         <v>3378</v>
       </c>
@@ -28650,9 +28924,15 @@
       <c r="B855" s="4" t="s">
         <v>2944</v>
       </c>
-      <c r="C855" s="11"/>
-      <c r="D855" s="4"/>
-      <c r="E855" s="12"/>
+      <c r="C855" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="D855" s="4" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E855" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F855" s="4" t="s">
         <v>3379</v>
       </c>
@@ -28664,9 +28944,15 @@
       <c r="B856" s="4" t="s">
         <v>2945</v>
       </c>
-      <c r="C856" s="11"/>
-      <c r="D856" s="4"/>
-      <c r="E856" s="12"/>
+      <c r="C856" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="D856" s="4" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E856" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F856" s="4" t="s">
         <v>2478</v>
       </c>
@@ -28678,9 +28964,15 @@
       <c r="B857" s="4" t="s">
         <v>2946</v>
       </c>
-      <c r="C857" s="11"/>
-      <c r="D857" s="4"/>
-      <c r="E857" s="12"/>
+      <c r="C857" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="D857" s="4" t="s">
+        <v>1037</v>
+      </c>
+      <c r="E857" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F857" s="4" t="s">
         <v>2479</v>
       </c>
@@ -28692,9 +28984,15 @@
       <c r="B858" s="4" t="s">
         <v>2947</v>
       </c>
-      <c r="C858" s="11"/>
-      <c r="D858" s="4"/>
-      <c r="E858" s="12"/>
+      <c r="C858" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="D858" s="4" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E858" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F858" s="4" t="s">
         <v>2480</v>
       </c>
@@ -29266,9 +29564,15 @@
       <c r="B887" s="4" t="s">
         <v>2976</v>
       </c>
-      <c r="C887" s="11"/>
-      <c r="D887" s="4"/>
-      <c r="E887" s="12"/>
+      <c r="C887" s="4" t="s">
+        <v>962</v>
+      </c>
+      <c r="D887" s="4" t="s">
+        <v>973</v>
+      </c>
+      <c r="E887" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F887" s="4" t="s">
         <v>2507</v>
       </c>
@@ -29280,9 +29584,15 @@
       <c r="B888" s="4" t="s">
         <v>2977</v>
       </c>
-      <c r="C888" s="11"/>
-      <c r="D888" s="4"/>
-      <c r="E888" s="12"/>
+      <c r="C888" s="4" t="s">
+        <v>962</v>
+      </c>
+      <c r="D888" s="4" t="s">
+        <v>970</v>
+      </c>
+      <c r="E888" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F888" s="4" t="s">
         <v>2508</v>
       </c>
@@ -29294,9 +29604,15 @@
       <c r="B889" s="4" t="s">
         <v>2978</v>
       </c>
-      <c r="C889" s="11"/>
-      <c r="D889" s="4"/>
-      <c r="E889" s="12"/>
+      <c r="C889" s="4" t="s">
+        <v>962</v>
+      </c>
+      <c r="D889" s="4" t="s">
+        <v>971</v>
+      </c>
+      <c r="E889" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F889" s="4" t="s">
         <v>2509</v>
       </c>
@@ -29308,9 +29624,15 @@
       <c r="B890" s="4" t="s">
         <v>2979</v>
       </c>
-      <c r="C890" s="11"/>
-      <c r="D890" s="4"/>
-      <c r="E890" s="12"/>
+      <c r="C890" s="4" t="s">
+        <v>1906</v>
+      </c>
+      <c r="D890" s="4" t="s">
+        <v>1968</v>
+      </c>
+      <c r="E890" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F890" s="4" t="s">
         <v>2510</v>
       </c>
@@ -29322,9 +29644,15 @@
       <c r="B891" s="4" t="s">
         <v>2980</v>
       </c>
-      <c r="C891" s="11"/>
-      <c r="D891" s="4"/>
-      <c r="E891" s="12"/>
+      <c r="C891" s="4" t="s">
+        <v>1906</v>
+      </c>
+      <c r="D891" s="4" t="s">
+        <v>1967</v>
+      </c>
+      <c r="E891" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F891" s="4" t="s">
         <v>2511</v>
       </c>
@@ -29336,9 +29664,15 @@
       <c r="B892" s="4" t="s">
         <v>2981</v>
       </c>
-      <c r="C892" s="11"/>
-      <c r="D892" s="4"/>
-      <c r="E892" s="12"/>
+      <c r="C892" s="4" t="s">
+        <v>1906</v>
+      </c>
+      <c r="D892" s="4" t="s">
+        <v>2400</v>
+      </c>
+      <c r="E892" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F892" s="4" t="s">
         <v>2512</v>
       </c>
@@ -29350,9 +29684,15 @@
       <c r="B893" s="4" t="s">
         <v>2982</v>
       </c>
-      <c r="C893" s="11"/>
-      <c r="D893" s="4"/>
-      <c r="E893" s="12"/>
+      <c r="C893" s="4" t="s">
+        <v>1906</v>
+      </c>
+      <c r="D893" s="4" t="s">
+        <v>2401</v>
+      </c>
+      <c r="E893" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F893" s="4" t="s">
         <v>2513</v>
       </c>
@@ -29364,9 +29704,15 @@
       <c r="B894" s="4" t="s">
         <v>2983</v>
       </c>
-      <c r="C894" s="11"/>
-      <c r="D894" s="4"/>
-      <c r="E894" s="12"/>
+      <c r="C894" s="4" t="s">
+        <v>1906</v>
+      </c>
+      <c r="D894" s="4" t="s">
+        <v>2402</v>
+      </c>
+      <c r="E894" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F894" s="4" t="s">
         <v>2514</v>
       </c>
@@ -29378,9 +29724,15 @@
       <c r="B895" s="4" t="s">
         <v>2984</v>
       </c>
-      <c r="C895" s="11"/>
-      <c r="D895" s="4"/>
-      <c r="E895" s="12"/>
+      <c r="C895" s="4" t="s">
+        <v>1906</v>
+      </c>
+      <c r="D895" s="4" t="s">
+        <v>2403</v>
+      </c>
+      <c r="E895" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F895" s="4" t="s">
         <v>2515</v>
       </c>
@@ -29392,9 +29744,15 @@
       <c r="B896" s="4" t="s">
         <v>2985</v>
       </c>
-      <c r="C896" s="11"/>
-      <c r="D896" s="4"/>
-      <c r="E896" s="12"/>
+      <c r="C896" s="4" t="s">
+        <v>1906</v>
+      </c>
+      <c r="D896" s="4" t="s">
+        <v>1957</v>
+      </c>
+      <c r="E896" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F896" s="4" t="s">
         <v>2516</v>
       </c>
@@ -29406,9 +29764,15 @@
       <c r="B897" s="4" t="s">
         <v>2986</v>
       </c>
-      <c r="C897" s="11"/>
-      <c r="D897" s="4"/>
-      <c r="E897" s="12"/>
+      <c r="C897" s="4" t="s">
+        <v>1906</v>
+      </c>
+      <c r="D897" s="4" t="s">
+        <v>2404</v>
+      </c>
+      <c r="E897" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F897" s="4" t="s">
         <v>2517</v>
       </c>
@@ -29420,9 +29784,15 @@
       <c r="B898" s="4" t="s">
         <v>2987</v>
       </c>
-      <c r="C898" s="11"/>
-      <c r="D898" s="4"/>
-      <c r="E898" s="12"/>
+      <c r="C898" s="4" t="s">
+        <v>1906</v>
+      </c>
+      <c r="D898" s="4" t="s">
+        <v>2405</v>
+      </c>
+      <c r="E898" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F898" s="4" t="s">
         <v>2518</v>
       </c>
@@ -29434,9 +29804,15 @@
       <c r="B899" s="4" t="s">
         <v>2988</v>
       </c>
-      <c r="C899" s="11"/>
-      <c r="D899" s="4"/>
-      <c r="E899" s="12"/>
+      <c r="C899" s="4" t="s">
+        <v>1906</v>
+      </c>
+      <c r="D899" s="4" t="s">
+        <v>2406</v>
+      </c>
+      <c r="E899" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F899" s="4" t="s">
         <v>2519</v>
       </c>
@@ -30568,11 +30944,13 @@
       <c r="B956" s="4" t="s">
         <v>3045</v>
       </c>
-      <c r="C956" s="11" t="s">
-        <v>3676</v>
-      </c>
-      <c r="D956" s="4"/>
-      <c r="E956" s="12" t="s">
+      <c r="C956" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D956" s="8" t="s">
+        <v>2108</v>
+      </c>
+      <c r="E956" s="8" t="s">
         <v>91</v>
       </c>
       <c r="F956" s="4" t="s">
@@ -30586,9 +30964,15 @@
       <c r="B957" s="4" t="s">
         <v>3046</v>
       </c>
-      <c r="C957" s="11"/>
-      <c r="D957" s="4"/>
-      <c r="E957" s="12"/>
+      <c r="C957" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D957" s="7" t="s">
+        <v>2082</v>
+      </c>
+      <c r="E957" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="F957" s="4" t="s">
         <v>2577</v>
       </c>
@@ -30600,9 +30984,15 @@
       <c r="B958" s="4" t="s">
         <v>3047</v>
       </c>
-      <c r="C958" s="11"/>
-      <c r="D958" s="4"/>
-      <c r="E958" s="12"/>
+      <c r="C958" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D958" s="8" t="s">
+        <v>2109</v>
+      </c>
+      <c r="E958" s="8" t="s">
+        <v>91</v>
+      </c>
       <c r="F958" s="4" t="s">
         <v>2578</v>
       </c>
@@ -30614,9 +31004,15 @@
       <c r="B959" s="4" t="s">
         <v>3048</v>
       </c>
-      <c r="C959" s="11"/>
-      <c r="D959" s="4"/>
-      <c r="E959" s="12"/>
+      <c r="C959" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D959" s="7" t="s">
+        <v>2083</v>
+      </c>
+      <c r="E959" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="F959" s="4" t="s">
         <v>2579</v>
       </c>
@@ -30628,9 +31024,15 @@
       <c r="B960" s="4" t="s">
         <v>3049</v>
       </c>
-      <c r="C960" s="11"/>
-      <c r="D960" s="4"/>
-      <c r="E960" s="12"/>
+      <c r="C960" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D960" s="8" t="s">
+        <v>2110</v>
+      </c>
+      <c r="E960" s="8" t="s">
+        <v>91</v>
+      </c>
       <c r="F960" s="4" t="s">
         <v>2580</v>
       </c>
@@ -30642,9 +31044,15 @@
       <c r="B961" s="4" t="s">
         <v>3050</v>
       </c>
-      <c r="C961" s="11"/>
-      <c r="D961" s="4"/>
-      <c r="E961" s="12"/>
+      <c r="C961" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D961" s="7" t="s">
+        <v>2084</v>
+      </c>
+      <c r="E961" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="F961" s="4" t="s">
         <v>2581</v>
       </c>
@@ -30656,9 +31064,15 @@
       <c r="B962" s="4" t="s">
         <v>3051</v>
       </c>
-      <c r="C962" s="11"/>
-      <c r="D962" s="4"/>
-      <c r="E962" s="12"/>
+      <c r="C962" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D962" s="8" t="s">
+        <v>2111</v>
+      </c>
+      <c r="E962" s="8" t="s">
+        <v>91</v>
+      </c>
       <c r="F962" s="4" t="s">
         <v>2582</v>
       </c>
@@ -30670,9 +31084,15 @@
       <c r="B963" s="4" t="s">
         <v>3052</v>
       </c>
-      <c r="C963" s="11"/>
-      <c r="D963" s="4"/>
-      <c r="E963" s="12"/>
+      <c r="C963" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D963" s="7" t="s">
+        <v>2085</v>
+      </c>
+      <c r="E963" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="F963" s="4" t="s">
         <v>2583</v>
       </c>
@@ -30684,9 +31104,15 @@
       <c r="B964" s="4" t="s">
         <v>3053</v>
       </c>
-      <c r="C964" s="11"/>
-      <c r="D964" s="4"/>
-      <c r="E964" s="12"/>
+      <c r="C964" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D964" s="8" t="s">
+        <v>2112</v>
+      </c>
+      <c r="E964" s="8" t="s">
+        <v>91</v>
+      </c>
       <c r="F964" s="4" t="s">
         <v>2584</v>
       </c>
@@ -30698,9 +31124,15 @@
       <c r="B965" s="4" t="s">
         <v>3054</v>
       </c>
-      <c r="C965" s="11"/>
-      <c r="D965" s="4"/>
-      <c r="E965" s="12"/>
+      <c r="C965" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D965" s="7" t="s">
+        <v>2086</v>
+      </c>
+      <c r="E965" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="F965" s="4" t="s">
         <v>2585</v>
       </c>
@@ -30712,9 +31144,15 @@
       <c r="B966" s="4" t="s">
         <v>3055</v>
       </c>
-      <c r="C966" s="11"/>
-      <c r="D966" s="4"/>
-      <c r="E966" s="12"/>
+      <c r="C966" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D966" s="8" t="s">
+        <v>2113</v>
+      </c>
+      <c r="E966" s="8" t="s">
+        <v>91</v>
+      </c>
       <c r="F966" s="4" t="s">
         <v>2586</v>
       </c>
@@ -30726,9 +31164,15 @@
       <c r="B967" s="4" t="s">
         <v>3056</v>
       </c>
-      <c r="C967" s="11"/>
-      <c r="D967" s="4"/>
-      <c r="E967" s="12"/>
+      <c r="C967" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D967" s="7" t="s">
+        <v>2087</v>
+      </c>
+      <c r="E967" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="F967" s="4" t="s">
         <v>2587</v>
       </c>
@@ -31860,9 +32304,15 @@
       <c r="B1024" s="4" t="s">
         <v>3113</v>
       </c>
-      <c r="C1024" s="11"/>
-      <c r="D1024" s="4"/>
-      <c r="E1024" s="12"/>
+      <c r="C1024" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D1024" s="7" t="s">
+        <v>2087</v>
+      </c>
+      <c r="E1024" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="F1024" s="4" t="s">
         <v>2644</v>
       </c>
@@ -31874,9 +32324,15 @@
       <c r="B1025" s="4" t="s">
         <v>3114</v>
       </c>
-      <c r="C1025" s="11"/>
-      <c r="D1025" s="4"/>
-      <c r="E1025" s="12"/>
+      <c r="C1025" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D1025" s="7" t="s">
+        <v>2087</v>
+      </c>
+      <c r="E1025" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="F1025" s="4" t="s">
         <v>2645</v>
       </c>
@@ -31888,9 +32344,15 @@
       <c r="B1026" s="4" t="s">
         <v>3115</v>
       </c>
-      <c r="C1026" s="11"/>
-      <c r="D1026" s="4"/>
-      <c r="E1026" s="12"/>
+      <c r="C1026" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D1026" s="7" t="s">
+        <v>2087</v>
+      </c>
+      <c r="E1026" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="F1026" s="4" t="s">
         <v>2646</v>
       </c>
@@ -31902,9 +32364,15 @@
       <c r="B1027" s="4" t="s">
         <v>3116</v>
       </c>
-      <c r="C1027" s="11"/>
-      <c r="D1027" s="4"/>
-      <c r="E1027" s="12"/>
+      <c r="C1027" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D1027" s="7" t="s">
+        <v>2087</v>
+      </c>
+      <c r="E1027" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="F1027" s="4" t="s">
         <v>2647</v>
       </c>
@@ -31916,9 +32384,15 @@
       <c r="B1028" s="4" t="s">
         <v>3117</v>
       </c>
-      <c r="C1028" s="11"/>
-      <c r="D1028" s="4"/>
-      <c r="E1028" s="12"/>
+      <c r="C1028" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D1028" s="7" t="s">
+        <v>2087</v>
+      </c>
+      <c r="E1028" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="F1028" s="4" t="s">
         <v>2648</v>
       </c>
@@ -32230,9 +32704,15 @@
       <c r="B1044" s="4" t="s">
         <v>3133</v>
       </c>
-      <c r="C1044" s="11"/>
-      <c r="D1044" s="4"/>
-      <c r="E1044" s="12"/>
+      <c r="C1044" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="D1044" s="4" t="s">
+        <v>949</v>
+      </c>
+      <c r="E1044" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F1044" s="4" t="s">
         <v>3373</v>
       </c>
@@ -32244,9 +32724,15 @@
       <c r="B1045" s="4" t="s">
         <v>3134</v>
       </c>
-      <c r="C1045" s="11"/>
-      <c r="D1045" s="4"/>
-      <c r="E1045" s="12"/>
+      <c r="C1045" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="D1045" s="4" t="s">
+        <v>950</v>
+      </c>
+      <c r="E1045" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F1045" s="4" t="s">
         <v>3374</v>
       </c>
@@ -32258,9 +32744,15 @@
       <c r="B1046" s="4" t="s">
         <v>3135</v>
       </c>
-      <c r="C1046" s="11"/>
-      <c r="D1046" s="4"/>
-      <c r="E1046" s="12"/>
+      <c r="C1046" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="D1046" s="4" t="s">
+        <v>951</v>
+      </c>
+      <c r="E1046" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F1046" s="4" t="s">
         <v>3375</v>
       </c>
@@ -32272,9 +32764,15 @@
       <c r="B1047" s="4" t="s">
         <v>3136</v>
       </c>
-      <c r="C1047" s="11"/>
-      <c r="D1047" s="4"/>
-      <c r="E1047" s="12"/>
+      <c r="C1047" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="D1047" s="4" t="s">
+        <v>952</v>
+      </c>
+      <c r="E1047" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F1047" s="4" t="s">
         <v>3376</v>
       </c>
@@ -32286,9 +32784,15 @@
       <c r="B1048" s="4" t="s">
         <v>3137</v>
       </c>
-      <c r="C1048" s="11"/>
-      <c r="D1048" s="4"/>
-      <c r="E1048" s="12"/>
+      <c r="C1048" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="D1048" s="4" t="s">
+        <v>957</v>
+      </c>
+      <c r="E1048" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F1048" s="4" t="s">
         <v>3377</v>
       </c>
@@ -32300,9 +32804,15 @@
       <c r="B1049" s="4" t="s">
         <v>3138</v>
       </c>
-      <c r="C1049" s="11"/>
-      <c r="D1049" s="4"/>
-      <c r="E1049" s="12"/>
+      <c r="C1049" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="D1049" s="4" t="s">
+        <v>958</v>
+      </c>
+      <c r="E1049" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F1049" s="4" t="s">
         <v>2664</v>
       </c>
@@ -32314,9 +32824,15 @@
       <c r="B1050" s="4" t="s">
         <v>3139</v>
       </c>
-      <c r="C1050" s="11"/>
-      <c r="D1050" s="4"/>
-      <c r="E1050" s="12"/>
+      <c r="C1050" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="D1050" s="4" t="s">
+        <v>959</v>
+      </c>
+      <c r="E1050" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F1050" s="4" t="s">
         <v>2665</v>
       </c>
@@ -32328,9 +32844,15 @@
       <c r="B1051" s="4" t="s">
         <v>3140</v>
       </c>
-      <c r="C1051" s="11"/>
-      <c r="D1051" s="4"/>
-      <c r="E1051" s="12"/>
+      <c r="C1051" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="D1051" s="4" t="s">
+        <v>960</v>
+      </c>
+      <c r="E1051" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F1051" s="4" t="s">
         <v>2666</v>
       </c>
@@ -32342,9 +32864,15 @@
       <c r="B1052" s="4" t="s">
         <v>3141</v>
       </c>
-      <c r="C1052" s="11"/>
-      <c r="D1052" s="4"/>
-      <c r="E1052" s="12"/>
+      <c r="C1052" s="4" t="s">
+        <v>2278</v>
+      </c>
+      <c r="D1052" s="4" t="s">
+        <v>2272</v>
+      </c>
+      <c r="E1052" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1052" s="4" t="s">
         <v>2667</v>
       </c>
@@ -32356,9 +32884,15 @@
       <c r="B1053" s="4" t="s">
         <v>3142</v>
       </c>
-      <c r="C1053" s="11"/>
-      <c r="D1053" s="4"/>
-      <c r="E1053" s="12"/>
+      <c r="C1053" s="4" t="s">
+        <v>2278</v>
+      </c>
+      <c r="D1053" s="4" t="s">
+        <v>2274</v>
+      </c>
+      <c r="E1053" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1053" s="4" t="s">
         <v>2668</v>
       </c>
@@ -32370,9 +32904,15 @@
       <c r="B1054" s="4" t="s">
         <v>3143</v>
       </c>
-      <c r="C1054" s="11"/>
-      <c r="D1054" s="4"/>
-      <c r="E1054" s="12"/>
+      <c r="C1054" s="4" t="s">
+        <v>2278</v>
+      </c>
+      <c r="D1054" s="4" t="s">
+        <v>2273</v>
+      </c>
+      <c r="E1054" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1054" s="4" t="s">
         <v>2669</v>
       </c>
@@ -32384,9 +32924,15 @@
       <c r="B1055" s="4" t="s">
         <v>3144</v>
       </c>
-      <c r="C1055" s="11"/>
-      <c r="D1055" s="4"/>
-      <c r="E1055" s="12"/>
+      <c r="C1055" s="4" t="s">
+        <v>2278</v>
+      </c>
+      <c r="D1055" s="4" t="s">
+        <v>2275</v>
+      </c>
+      <c r="E1055" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1055" s="4" t="s">
         <v>2670</v>
       </c>
@@ -32398,9 +32944,15 @@
       <c r="B1056" s="4" t="s">
         <v>3145</v>
       </c>
-      <c r="C1056" s="11"/>
-      <c r="D1056" s="4"/>
-      <c r="E1056" s="12"/>
+      <c r="C1056" s="4" t="s">
+        <v>2278</v>
+      </c>
+      <c r="D1056" s="4" t="s">
+        <v>2276</v>
+      </c>
+      <c r="E1056" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1056" s="4" t="s">
         <v>2671</v>
       </c>
@@ -32412,9 +32964,15 @@
       <c r="B1057" s="4" t="s">
         <v>3146</v>
       </c>
-      <c r="C1057" s="11"/>
-      <c r="D1057" s="4"/>
-      <c r="E1057" s="12"/>
+      <c r="C1057" s="4" t="s">
+        <v>2278</v>
+      </c>
+      <c r="D1057" s="4" t="s">
+        <v>2277</v>
+      </c>
+      <c r="E1057" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1057" s="4" t="s">
         <v>2672</v>
       </c>
@@ -32426,9 +32984,15 @@
       <c r="B1058" s="4" t="s">
         <v>3147</v>
       </c>
-      <c r="C1058" s="11"/>
-      <c r="D1058" s="4"/>
-      <c r="E1058" s="12"/>
+      <c r="C1058" s="4" t="s">
+        <v>2278</v>
+      </c>
+      <c r="D1058" s="4" t="s">
+        <v>2289</v>
+      </c>
+      <c r="E1058" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1058" s="4" t="s">
         <v>2673</v>
       </c>
@@ -32440,9 +33004,15 @@
       <c r="B1059" s="4" t="s">
         <v>3148</v>
       </c>
-      <c r="C1059" s="11"/>
-      <c r="D1059" s="4"/>
-      <c r="E1059" s="12"/>
+      <c r="C1059" s="4" t="s">
+        <v>2278</v>
+      </c>
+      <c r="D1059" s="4" t="s">
+        <v>2290</v>
+      </c>
+      <c r="E1059" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1059" s="4" t="s">
         <v>2674</v>
       </c>
@@ -32454,9 +33024,15 @@
       <c r="B1060" s="4" t="s">
         <v>3149</v>
       </c>
-      <c r="C1060" s="11"/>
-      <c r="D1060" s="4"/>
-      <c r="E1060" s="12"/>
+      <c r="C1060" s="4" t="s">
+        <v>2278</v>
+      </c>
+      <c r="D1060" s="4" t="s">
+        <v>2293</v>
+      </c>
+      <c r="E1060" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1060" s="4" t="s">
         <v>2675</v>
       </c>
@@ -32468,9 +33044,15 @@
       <c r="B1061" s="4" t="s">
         <v>3150</v>
       </c>
-      <c r="C1061" s="11"/>
-      <c r="D1061" s="4"/>
-      <c r="E1061" s="12"/>
+      <c r="C1061" s="4" t="s">
+        <v>2278</v>
+      </c>
+      <c r="D1061" s="4" t="s">
+        <v>2294</v>
+      </c>
+      <c r="E1061" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1061" s="4" t="s">
         <v>2676</v>
       </c>
@@ -32482,9 +33064,15 @@
       <c r="B1062" s="4" t="s">
         <v>3151</v>
       </c>
-      <c r="C1062" s="11"/>
-      <c r="D1062" s="4"/>
-      <c r="E1062" s="12"/>
+      <c r="C1062" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="D1062" s="4" t="s">
+        <v>960</v>
+      </c>
+      <c r="E1062" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F1062" s="4" t="s">
         <v>2677</v>
       </c>
@@ -32496,9 +33084,15 @@
       <c r="B1063" s="4" t="s">
         <v>3152</v>
       </c>
-      <c r="C1063" s="11"/>
-      <c r="D1063" s="4"/>
-      <c r="E1063" s="12"/>
+      <c r="C1063" s="4" t="s">
+        <v>2278</v>
+      </c>
+      <c r="D1063" s="4" t="s">
+        <v>2272</v>
+      </c>
+      <c r="E1063" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1063" s="4" t="s">
         <v>2678</v>
       </c>
@@ -36368,9 +36962,15 @@
       <c r="B1257" s="4" t="s">
         <v>3346</v>
       </c>
-      <c r="C1257" s="11"/>
-      <c r="D1257" s="4"/>
-      <c r="E1257" s="12"/>
+      <c r="C1257" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1257" s="10" t="s">
+        <v>2165</v>
+      </c>
+      <c r="E1257" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1257" s="4" t="s">
         <v>2871</v>
       </c>
@@ -36382,9 +36982,15 @@
       <c r="B1258" s="4" t="s">
         <v>3347</v>
       </c>
-      <c r="C1258" s="11"/>
-      <c r="D1258" s="4"/>
-      <c r="E1258" s="12"/>
+      <c r="C1258" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1258" s="10" t="s">
+        <v>2164</v>
+      </c>
+      <c r="E1258" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1258" s="4" t="s">
         <v>2872</v>
       </c>
@@ -36396,9 +37002,15 @@
       <c r="B1259" s="4" t="s">
         <v>3348</v>
       </c>
-      <c r="C1259" s="11"/>
-      <c r="D1259" s="4"/>
-      <c r="E1259" s="12"/>
+      <c r="C1259" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1259" s="10" t="s">
+        <v>2170</v>
+      </c>
+      <c r="E1259" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1259" s="6" t="s">
         <v>2873</v>
       </c>
@@ -36410,9 +37022,15 @@
       <c r="B1260" s="4" t="s">
         <v>3349</v>
       </c>
-      <c r="C1260" s="11"/>
-      <c r="D1260" s="4"/>
-      <c r="E1260" s="12"/>
+      <c r="C1260" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1260" s="10" t="s">
+        <v>2171</v>
+      </c>
+      <c r="E1260" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1260" s="4" t="s">
         <v>2874</v>
       </c>
@@ -36424,9 +37042,15 @@
       <c r="B1261" s="4" t="s">
         <v>3350</v>
       </c>
-      <c r="C1261" s="11"/>
-      <c r="D1261" s="4"/>
-      <c r="E1261" s="12"/>
+      <c r="C1261" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1261" s="10" t="s">
+        <v>2178</v>
+      </c>
+      <c r="E1261" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1261" s="4" t="s">
         <v>2875</v>
       </c>
@@ -36438,9 +37062,15 @@
       <c r="B1262" s="4" t="s">
         <v>3351</v>
       </c>
-      <c r="C1262" s="11"/>
-      <c r="D1262" s="4"/>
-      <c r="E1262" s="12"/>
+      <c r="C1262" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1262" s="10" t="s">
+        <v>2179</v>
+      </c>
+      <c r="E1262" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1262" s="4" t="s">
         <v>2876</v>
       </c>
@@ -36452,9 +37082,15 @@
       <c r="B1263" s="4" t="s">
         <v>3352</v>
       </c>
-      <c r="C1263" s="11"/>
-      <c r="D1263" s="4"/>
-      <c r="E1263" s="12"/>
+      <c r="C1263" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1263" s="4" t="s">
+        <v>2182</v>
+      </c>
+      <c r="E1263" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1263" s="4" t="s">
         <v>2877</v>
       </c>
@@ -36466,9 +37102,15 @@
       <c r="B1264" s="4" t="s">
         <v>3353</v>
       </c>
-      <c r="C1264" s="11"/>
-      <c r="D1264" s="4"/>
-      <c r="E1264" s="12"/>
+      <c r="C1264" s="10" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D1264" s="10" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E1264" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1264" s="4" t="s">
         <v>2878</v>
       </c>
@@ -36480,9 +37122,15 @@
       <c r="B1265" s="4" t="s">
         <v>3354</v>
       </c>
-      <c r="C1265" s="11"/>
-      <c r="D1265" s="4"/>
-      <c r="E1265" s="12"/>
+      <c r="C1265" s="10" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D1265" s="10" t="s">
+        <v>2250</v>
+      </c>
+      <c r="E1265" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1265" s="4" t="s">
         <v>2879</v>
       </c>
@@ -36494,9 +37142,15 @@
       <c r="B1266" s="4" t="s">
         <v>3355</v>
       </c>
-      <c r="C1266" s="11"/>
-      <c r="D1266" s="4"/>
-      <c r="E1266" s="12"/>
+      <c r="C1266" s="10" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D1266" s="10" t="s">
+        <v>2227</v>
+      </c>
+      <c r="E1266" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1266" s="4" t="s">
         <v>2880</v>
       </c>
@@ -36508,9 +37162,15 @@
       <c r="B1267" s="4" t="s">
         <v>3356</v>
       </c>
-      <c r="C1267" s="11"/>
-      <c r="D1267" s="4"/>
-      <c r="E1267" s="12"/>
+      <c r="C1267" s="10" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D1267" s="10" t="s">
+        <v>2228</v>
+      </c>
+      <c r="E1267" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1267" s="4" t="s">
         <v>2881</v>
       </c>
@@ -36522,9 +37182,15 @@
       <c r="B1268" s="4" t="s">
         <v>3357</v>
       </c>
-      <c r="C1268" s="11"/>
-      <c r="D1268" s="4"/>
-      <c r="E1268" s="12"/>
+      <c r="C1268" s="10" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D1268" s="10" t="s">
+        <v>2229</v>
+      </c>
+      <c r="E1268" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1268" s="4" t="s">
         <v>2882</v>
       </c>
@@ -36536,9 +37202,15 @@
       <c r="B1269" s="4" t="s">
         <v>3358</v>
       </c>
-      <c r="C1269" s="11"/>
-      <c r="D1269" s="4"/>
-      <c r="E1269" s="12"/>
+      <c r="C1269" s="10" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D1269" s="10" t="s">
+        <v>2230</v>
+      </c>
+      <c r="E1269" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1269" s="4" t="s">
         <v>2883</v>
       </c>
@@ -36550,9 +37222,15 @@
       <c r="B1270" s="4" t="s">
         <v>3359</v>
       </c>
-      <c r="C1270" s="11"/>
-      <c r="D1270" s="4"/>
-      <c r="E1270" s="12"/>
+      <c r="C1270" s="10" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D1270" s="10" t="s">
+        <v>2231</v>
+      </c>
+      <c r="E1270" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1270" s="4" t="s">
         <v>2884</v>
       </c>
@@ -36564,9 +37242,15 @@
       <c r="B1271" s="4" t="s">
         <v>3360</v>
       </c>
-      <c r="C1271" s="11"/>
-      <c r="D1271" s="4"/>
-      <c r="E1271" s="12"/>
+      <c r="C1271" s="10" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D1271" s="10" t="s">
+        <v>2232</v>
+      </c>
+      <c r="E1271" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1271" s="4" t="s">
         <v>2885</v>
       </c>
@@ -36578,9 +37262,15 @@
       <c r="B1272" s="4" t="s">
         <v>3361</v>
       </c>
-      <c r="C1272" s="11"/>
-      <c r="D1272" s="4"/>
-      <c r="E1272" s="12"/>
+      <c r="C1272" s="10" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D1272" s="10" t="s">
+        <v>2233</v>
+      </c>
+      <c r="E1272" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1272" s="4" t="s">
         <v>2886</v>
       </c>
@@ -36592,9 +37282,15 @@
       <c r="B1273" s="4" t="s">
         <v>3362</v>
       </c>
-      <c r="C1273" s="11"/>
-      <c r="D1273" s="4"/>
-      <c r="E1273" s="12"/>
+      <c r="C1273" s="10" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D1273" s="10" t="s">
+        <v>2234</v>
+      </c>
+      <c r="E1273" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1273" s="4" t="s">
         <v>2887</v>
       </c>
@@ -36606,9 +37302,15 @@
       <c r="B1274" s="4" t="s">
         <v>3363</v>
       </c>
-      <c r="C1274" s="11"/>
-      <c r="D1274" s="4"/>
-      <c r="E1274" s="12"/>
+      <c r="C1274" s="10" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D1274" s="10" t="s">
+        <v>2235</v>
+      </c>
+      <c r="E1274" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1274" s="4" t="s">
         <v>2888</v>
       </c>
@@ -36620,9 +37322,15 @@
       <c r="B1275" s="4" t="s">
         <v>3364</v>
       </c>
-      <c r="C1275" s="11"/>
-      <c r="D1275" s="4"/>
-      <c r="E1275" s="12"/>
+      <c r="C1275" s="10" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D1275" s="10" t="s">
+        <v>2236</v>
+      </c>
+      <c r="E1275" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1275" s="4" t="s">
         <v>2889</v>
       </c>
@@ -36634,9 +37342,15 @@
       <c r="B1276" s="4" t="s">
         <v>3365</v>
       </c>
-      <c r="C1276" s="11"/>
-      <c r="D1276" s="4"/>
-      <c r="E1276" s="12"/>
+      <c r="C1276" s="10" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D1276" s="10" t="s">
+        <v>2237</v>
+      </c>
+      <c r="E1276" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1276" s="4" t="s">
         <v>2890</v>
       </c>
@@ -36648,9 +37362,15 @@
       <c r="B1277" s="4" t="s">
         <v>3366</v>
       </c>
-      <c r="C1277" s="11"/>
-      <c r="D1277" s="4"/>
-      <c r="E1277" s="12"/>
+      <c r="C1277" s="10" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D1277" s="10" t="s">
+        <v>2238</v>
+      </c>
+      <c r="E1277" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1277" s="4" t="s">
         <v>2891</v>
       </c>
@@ -36662,9 +37382,15 @@
       <c r="B1278" s="4" t="s">
         <v>3367</v>
       </c>
-      <c r="C1278" s="11"/>
-      <c r="D1278" s="4"/>
-      <c r="E1278" s="12"/>
+      <c r="C1278" s="10" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D1278" s="10" t="s">
+        <v>2239</v>
+      </c>
+      <c r="E1278" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1278" s="4" t="s">
         <v>2892</v>
       </c>
@@ -36676,9 +37402,15 @@
       <c r="B1279" s="4" t="s">
         <v>3368</v>
       </c>
-      <c r="C1279" s="11"/>
-      <c r="D1279" s="4"/>
-      <c r="E1279" s="12"/>
+      <c r="C1279" s="10" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D1279" s="10" t="s">
+        <v>2240</v>
+      </c>
+      <c r="E1279" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1279" s="4" t="s">
         <v>2893</v>
       </c>
@@ -36690,9 +37422,15 @@
       <c r="B1280" s="4" t="s">
         <v>3369</v>
       </c>
-      <c r="C1280" s="11"/>
-      <c r="D1280" s="4"/>
-      <c r="E1280" s="12"/>
+      <c r="C1280" s="10" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D1280" s="10" t="s">
+        <v>2241</v>
+      </c>
+      <c r="E1280" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1280" s="4" t="s">
         <v>2894</v>
       </c>
@@ -36704,9 +37442,15 @@
       <c r="B1281" s="4" t="s">
         <v>3370</v>
       </c>
-      <c r="C1281" s="11"/>
-      <c r="D1281" s="4"/>
-      <c r="E1281" s="12"/>
+      <c r="C1281" s="10" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D1281" s="10" t="s">
+        <v>2242</v>
+      </c>
+      <c r="E1281" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1281" s="4" t="s">
         <v>2895</v>
       </c>
@@ -36718,9 +37462,15 @@
       <c r="B1282" s="4" t="s">
         <v>3371</v>
       </c>
-      <c r="C1282" s="11"/>
-      <c r="D1282" s="4"/>
-      <c r="E1282" s="12"/>
+      <c r="C1282" s="10" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D1282" s="10" t="s">
+        <v>2243</v>
+      </c>
+      <c r="E1282" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1282" s="4" t="s">
         <v>2896</v>
       </c>
@@ -36732,9 +37482,15 @@
       <c r="B1283" s="4" t="s">
         <v>3372</v>
       </c>
-      <c r="C1283" s="13"/>
-      <c r="D1283" s="10"/>
-      <c r="E1283" s="14"/>
+      <c r="C1283" s="10" t="s">
+        <v>1984</v>
+      </c>
+      <c r="D1283" s="10" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E1283" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F1283" s="10" t="s">
         <v>2897</v>
       </c>
@@ -37264,4 +38020,261 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{713C69A7-386E-4068-A295-FC2A04A02B4E}">
+  <dimension ref="C4:E25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="3:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="C4" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>2108</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="C5" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>2082</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="C6" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>2109</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="C7" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>2083</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="C8" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>2110</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="C9" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>2084</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="C10" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>2111</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="C11" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>2085</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="C12" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>2112</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="C13" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>2086</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="C14" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>2113</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="C15" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>2087</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="C16" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>2114</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="C17" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>2088</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="C18" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>2115</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="C19" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>2089</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="C20" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>2116</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="C21" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>2090</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="C22" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>2091</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="C23" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>2092</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="C24" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>2093</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="C25" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>2094</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added cases for email ric
</commit_message>
<xml_diff>
--- a/LYNX_Automation/src/test/resources/TestData/Test_Data.xlsx
+++ b/LYNX_Automation/src/test/resources/TestData/Test_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X023840\git\Fastwire_Sikuli\LYNX_Automation\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E1C208-0446-46A3-99B4-1057C6E3076E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CC9FEE-E06B-4003-9997-95A5660CF029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7917" uniqueCount="3676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7971" uniqueCount="3695">
   <si>
     <t>RunTest</t>
   </si>
@@ -11067,6 +11067,63 @@
   </si>
   <si>
     <t>Aim of the Script is to verify Whether selected company list, automations filters and web watchers retained in next session when user relaunches fastwire</t>
+  </si>
+  <si>
+    <t>VerifyEmailRIC</t>
+  </si>
+  <si>
+    <t>FW_UI_1309</t>
+  </si>
+  <si>
+    <t>FW_UI_1310</t>
+  </si>
+  <si>
+    <t>FW_UI_1311</t>
+  </si>
+  <si>
+    <t>FW_UI_1312</t>
+  </si>
+  <si>
+    <t>FW_UI_1313</t>
+  </si>
+  <si>
+    <t>FW_UI_1314</t>
+  </si>
+  <si>
+    <t>FW_UI_1315</t>
+  </si>
+  <si>
+    <t>FW_UI_1316</t>
+  </si>
+  <si>
+    <t>FW_UI_1317</t>
+  </si>
+  <si>
+    <t>zenergyreports,energyreports,iirenergy.com,S.BK</t>
+  </si>
+  <si>
+    <t>zUSDA Foreign Agricultural Service,FAS.USDA,service.govdelivery.com,S.BK</t>
+  </si>
+  <si>
+    <t>zUSDA Farm Service Agency,usdafarmers,public.govdelivery.com,S.BK</t>
+  </si>
+  <si>
+    <t>zIntercontinental Exchange,emailalerts-ir,theice.com,S.BK</t>
+  </si>
+  <si>
+    <t>zKiara King (ZA),Kiara.King,absa.africa,S.BK</t>
+  </si>
+  <si>
+    <t>zSilind'okuhle Khanyile (ZA),Silindokuhle.Khanyile,absa.africa,S.BK</t>
+  </si>
+  <si>
+    <t>zNokukhanya Masemola (ZA),Nokukhanya.Masemola,absa.africa,S.BK</t>
+  </si>
+  <si>
+    <t>zANZ Research,research,anz.com,S.BK</t>
+  </si>
+  <si>
+    <t>zICEFuturesEurope,ICEFuturesEurope.Circulars,ice.com,S.BK</t>
   </si>
 </sst>
 </file>
@@ -11209,7 +11266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -11269,6 +11326,15 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -11518,7 +11584,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CBB49106-BC95-4A00-9B23-0E30E5D20288}" name="Table2" displayName="Table2" ref="A1:F1309" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CBB49106-BC95-4A00-9B23-0E30E5D20288}" name="Table2" displayName="Table2" ref="A1:F1318" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E8C12C75-5AB5-4A43-A3C6-442932DE8960}" name="RunTest" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{2D0C15F7-7463-4837-A664-2CE60CA101D5}" name="TC_ID" dataDxfId="4"/>
@@ -11819,10 +11885,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F1309"/>
+  <dimension ref="A1:F1318"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" activeCellId="1" sqref="F19 F10"/>
+    <sheetView tabSelected="1" topLeftCell="A1307" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A1309" sqref="A1309:A1317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11859,7 +11925,7 @@
     </row>
     <row r="2" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>3430</v>
+        <v>2054</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>4</v>
@@ -11879,7 +11945,7 @@
     </row>
     <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>3430</v>
+        <v>2054</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -11899,7 +11965,7 @@
     </row>
     <row r="4" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>3430</v>
+        <v>2054</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>9</v>
@@ -11919,7 +11985,7 @@
     </row>
     <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>3430</v>
+        <v>2054</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>10</v>
@@ -11939,7 +12005,7 @@
     </row>
     <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>3430</v>
+        <v>2054</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>11</v>
@@ -11959,7 +12025,7 @@
     </row>
     <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>3430</v>
+        <v>2054</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>14</v>
@@ -11979,7 +12045,7 @@
     </row>
     <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>3430</v>
+        <v>2054</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>18</v>
@@ -11999,7 +12065,7 @@
     </row>
     <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>3430</v>
+        <v>2054</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>20</v>
@@ -12019,7 +12085,7 @@
     </row>
     <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>3430</v>
+        <v>2054</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>22</v>
@@ -12039,7 +12105,7 @@
     </row>
     <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>3430</v>
+        <v>2054</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>23</v>
@@ -28184,13 +28250,13 @@
       <c r="B818" s="4" t="s">
         <v>2907</v>
       </c>
-      <c r="C818" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="D818" s="4" t="s">
-        <v>2086</v>
-      </c>
-      <c r="E818" s="4" t="s">
+      <c r="C818" s="22" t="s">
+        <v>3676</v>
+      </c>
+      <c r="D818" s="21" t="s">
+        <v>3686</v>
+      </c>
+      <c r="E818" s="23" t="s">
         <v>91</v>
       </c>
       <c r="F818" s="4" t="s">
@@ -28204,13 +28270,13 @@
       <c r="B819" s="4" t="s">
         <v>2908</v>
       </c>
-      <c r="C819" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="D819" s="4" t="s">
-        <v>2113</v>
-      </c>
-      <c r="E819" s="4" t="s">
+      <c r="C819" s="22" t="s">
+        <v>3676</v>
+      </c>
+      <c r="D819" s="21" t="s">
+        <v>3686</v>
+      </c>
+      <c r="E819" s="23" t="s">
         <v>91</v>
       </c>
       <c r="F819" s="4" t="s">
@@ -28224,13 +28290,13 @@
       <c r="B820" s="4" t="s">
         <v>2909</v>
       </c>
-      <c r="C820" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="D820" s="4" t="s">
-        <v>2087</v>
-      </c>
-      <c r="E820" s="4" t="s">
+      <c r="C820" s="22" t="s">
+        <v>3676</v>
+      </c>
+      <c r="D820" s="21" t="s">
+        <v>3686</v>
+      </c>
+      <c r="E820" s="23" t="s">
         <v>91</v>
       </c>
       <c r="F820" s="4" t="s">
@@ -38009,6 +38075,186 @@
       </c>
       <c r="F1309" s="17" t="s">
         <v>3675</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1310" s="4" t="s">
+        <v>2054</v>
+      </c>
+      <c r="B1310" s="10" t="s">
+        <v>3677</v>
+      </c>
+      <c r="C1310" s="22" t="s">
+        <v>3676</v>
+      </c>
+      <c r="D1310" s="21" t="s">
+        <v>3686</v>
+      </c>
+      <c r="E1310" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1310" s="21" t="s">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1311" s="4" t="s">
+        <v>2054</v>
+      </c>
+      <c r="B1311" s="10" t="s">
+        <v>3678</v>
+      </c>
+      <c r="C1311" s="22" t="s">
+        <v>3676</v>
+      </c>
+      <c r="D1311" s="21" t="s">
+        <v>3687</v>
+      </c>
+      <c r="E1311" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1311" s="21" t="s">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1312" s="4" t="s">
+        <v>2054</v>
+      </c>
+      <c r="B1312" s="10" t="s">
+        <v>3679</v>
+      </c>
+      <c r="C1312" s="22" t="s">
+        <v>3676</v>
+      </c>
+      <c r="D1312" s="21" t="s">
+        <v>3688</v>
+      </c>
+      <c r="E1312" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1312" s="21" t="s">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1313" s="4" t="s">
+        <v>2054</v>
+      </c>
+      <c r="B1313" s="10" t="s">
+        <v>3680</v>
+      </c>
+      <c r="C1313" s="22" t="s">
+        <v>3676</v>
+      </c>
+      <c r="D1313" s="21" t="s">
+        <v>3689</v>
+      </c>
+      <c r="E1313" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1313" s="21" t="s">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1314" s="4" t="s">
+        <v>2054</v>
+      </c>
+      <c r="B1314" s="10" t="s">
+        <v>3681</v>
+      </c>
+      <c r="C1314" s="22" t="s">
+        <v>3676</v>
+      </c>
+      <c r="D1314" s="21" t="s">
+        <v>3690</v>
+      </c>
+      <c r="E1314" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1314" s="21" t="s">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1315" s="4" t="s">
+        <v>2054</v>
+      </c>
+      <c r="B1315" s="10" t="s">
+        <v>3682</v>
+      </c>
+      <c r="C1315" s="22" t="s">
+        <v>3676</v>
+      </c>
+      <c r="D1315" s="21" t="s">
+        <v>3691</v>
+      </c>
+      <c r="E1315" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1315" s="21" t="s">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1316" s="4" t="s">
+        <v>2054</v>
+      </c>
+      <c r="B1316" s="10" t="s">
+        <v>3683</v>
+      </c>
+      <c r="C1316" s="22" t="s">
+        <v>3676</v>
+      </c>
+      <c r="D1316" s="21" t="s">
+        <v>3692</v>
+      </c>
+      <c r="E1316" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1316" s="21" t="s">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1317" s="4" t="s">
+        <v>2054</v>
+      </c>
+      <c r="B1317" s="10" t="s">
+        <v>3684</v>
+      </c>
+      <c r="C1317" s="22" t="s">
+        <v>3676</v>
+      </c>
+      <c r="D1317" s="21" t="s">
+        <v>3693</v>
+      </c>
+      <c r="E1317" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1317" s="21" t="s">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1318" s="21" t="s">
+        <v>3430</v>
+      </c>
+      <c r="B1318" s="10" t="s">
+        <v>3685</v>
+      </c>
+      <c r="C1318" s="22" t="s">
+        <v>3676</v>
+      </c>
+      <c r="D1318" s="21" t="s">
+        <v>3694</v>
+      </c>
+      <c r="E1318" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1318" s="21" t="s">
+        <v>2442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>